<commit_message>
Test Passed for createChange.py
</commit_message>
<xml_diff>
--- a/data_driver/Change_Request_List.xlsx
+++ b/data_driver/Change_Request_List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Change_List" sheetId="1" state="visible" r:id="rId1"/>
@@ -608,7 +608,7 @@
       </c>
       <c r="B2" s="8" t="inlineStr">
         <is>
-          <t>29-Jul-20</t>
+          <t>10-Aug-20</t>
         </is>
       </c>
       <c r="C2" s="7" t="inlineStr">
@@ -653,7 +653,7 @@
       </c>
       <c r="K2" s="11" t="inlineStr">
         <is>
-          <t>CRQ000000248819</t>
+          <t>CRQ000000249241</t>
         </is>
       </c>
       <c r="L2" s="11" t="inlineStr">
@@ -668,27 +668,27 @@
       </c>
       <c r="B3" s="8" t="inlineStr">
         <is>
-          <t>29-Jul-20</t>
+          <t>10-Aug-20</t>
         </is>
       </c>
       <c r="C3" s="7" t="inlineStr">
         <is>
-          <t>Md. Masudur Rahman</t>
+          <t>KM Jiaul Islam Jibon</t>
         </is>
       </c>
       <c r="D3" s="9" t="inlineStr">
         <is>
-          <t>Legacy</t>
+          <t>Operational</t>
         </is>
       </c>
       <c r="E3" s="9" t="inlineStr">
         <is>
-          <t>New Link instalation</t>
+          <t xml:space="preserve">TEST </t>
         </is>
       </c>
       <c r="F3" s="9" t="inlineStr">
         <is>
-          <t>NGSNG07,NGSNG57</t>
+          <t>MBKLR30,MBKLR27</t>
         </is>
       </c>
       <c r="G3" s="14" t="inlineStr">
@@ -708,17 +708,17 @@
       </c>
       <c r="J3" s="10" t="inlineStr">
         <is>
-          <t>e.co_Dhaka South</t>
+          <t>e.co_Dhaka Metro</t>
         </is>
       </c>
       <c r="K3" s="11" t="inlineStr">
         <is>
-          <t>CRQ000000248827</t>
+          <t>CRQ000000249243</t>
         </is>
       </c>
       <c r="L3" s="11" t="inlineStr">
         <is>
-          <t>Muhammad Shahed</t>
+          <t>Shahriar Mahbub</t>
         </is>
       </c>
     </row>
@@ -726,481 +726,129 @@
       <c r="A4" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="inlineStr">
-        <is>
-          <t>29-Jul-20</t>
-        </is>
-      </c>
-      <c r="C4" s="7" t="inlineStr">
-        <is>
-          <t>Md. Masudur Rahman</t>
-        </is>
-      </c>
-      <c r="D4" s="9" t="inlineStr">
-        <is>
-          <t>Operational</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="inlineStr">
-        <is>
-          <t>PAT activity</t>
-        </is>
-      </c>
-      <c r="F4" s="9" t="inlineStr">
-        <is>
-          <t>SYSDRB6,SYSDRA8</t>
-        </is>
-      </c>
-      <c r="G4" s="14" t="inlineStr">
-        <is>
-          <t>Service Effective</t>
-        </is>
-      </c>
-      <c r="H4" s="9" t="inlineStr">
-        <is>
-          <t>00:30 Minute</t>
-        </is>
-      </c>
-      <c r="I4" s="9" t="inlineStr">
-        <is>
-          <t>Sylhet</t>
-        </is>
-      </c>
-      <c r="J4" s="10" t="inlineStr">
-        <is>
-          <t>e.co_Sylhet</t>
-        </is>
-      </c>
-      <c r="K4" s="11" t="inlineStr">
-        <is>
-          <t>CRQ000000248831</t>
-        </is>
-      </c>
-      <c r="L4" s="11" t="inlineStr">
-        <is>
-          <t>Muhammad Shahed</t>
-        </is>
-      </c>
+      <c r="B4" s="8" t="n"/>
+      <c r="C4" s="7" t="n"/>
+      <c r="D4" s="9" t="n"/>
+      <c r="E4" s="9" t="n"/>
+      <c r="F4" s="9" t="n"/>
+      <c r="G4" s="14" t="n"/>
+      <c r="H4" s="9" t="n"/>
+      <c r="I4" s="9" t="n"/>
+      <c r="J4" s="10" t="n"/>
+      <c r="K4" s="11" t="n"/>
+      <c r="L4" s="11" t="n"/>
     </row>
     <row r="5" ht="15.75" customHeight="1" s="1">
       <c r="A5" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="inlineStr">
-        <is>
-          <t>29-Jul-20</t>
-        </is>
-      </c>
-      <c r="C5" s="7" t="inlineStr">
-        <is>
-          <t>Md. Masudur Rahman</t>
-        </is>
-      </c>
-      <c r="D5" s="9" t="inlineStr">
-        <is>
-          <t>DHAKA_MODERNIZATION</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RAU Release Udate </t>
-        </is>
-      </c>
-      <c r="F5" s="9" t="inlineStr">
-        <is>
-          <t>DHKHL05,DHKHL74</t>
-        </is>
-      </c>
-      <c r="G5" s="14" t="inlineStr">
-        <is>
-          <t>Service Effective</t>
-        </is>
-      </c>
-      <c r="H5" s="9" t="inlineStr">
-        <is>
-          <t>00:30 Minute</t>
-        </is>
-      </c>
-      <c r="I5" s="9" t="inlineStr">
-        <is>
-          <t>Dhaka</t>
-        </is>
-      </c>
-      <c r="J5" s="10" t="inlineStr">
-        <is>
-          <t>e.co_Dhaka Metro</t>
-        </is>
-      </c>
-      <c r="K5" s="11" t="inlineStr">
-        <is>
-          <t>CRQ000000248835</t>
-        </is>
-      </c>
-      <c r="L5" s="11" t="inlineStr">
-        <is>
-          <t>Muhammad Shahed</t>
-        </is>
-      </c>
+      <c r="B5" s="8" t="n"/>
+      <c r="C5" s="7" t="n"/>
+      <c r="D5" s="9" t="n"/>
+      <c r="E5" s="9" t="n"/>
+      <c r="F5" s="9" t="n"/>
+      <c r="G5" s="14" t="n"/>
+      <c r="H5" s="9" t="n"/>
+      <c r="I5" s="9" t="n"/>
+      <c r="J5" s="10" t="n"/>
+      <c r="K5" s="11" t="n"/>
+      <c r="L5" s="11" t="n"/>
     </row>
     <row r="6" ht="15.75" customHeight="1" s="1">
       <c r="A6" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="inlineStr">
-        <is>
-          <t>29-Jul-20</t>
-        </is>
-      </c>
-      <c r="C6" s="7" t="inlineStr">
-        <is>
-          <t>Md. Masudur Rahman</t>
-        </is>
-      </c>
-      <c r="D6" s="9" t="inlineStr">
-        <is>
-          <t>NCCD AbisoIP</t>
-        </is>
-      </c>
-      <c r="E6" s="9" t="inlineStr">
-        <is>
-          <t>Dismantle activity</t>
-        </is>
-      </c>
-      <c r="F6" s="9" t="inlineStr">
-        <is>
-          <t>SYGWN10,SYGWN13,SYGWN05,SYGWN01,SYSDR34</t>
-        </is>
-      </c>
-      <c r="G6" s="14" t="inlineStr">
-        <is>
-          <t>Non-Service Effective</t>
-        </is>
-      </c>
-      <c r="H6" s="9" t="inlineStr">
-        <is>
-          <t>00:00 Minute</t>
-        </is>
-      </c>
-      <c r="I6" s="9" t="inlineStr">
-        <is>
-          <t>Sylhet</t>
-        </is>
-      </c>
-      <c r="J6" s="10" t="inlineStr">
-        <is>
-          <t>e.co_Sylhet</t>
-        </is>
-      </c>
-      <c r="K6" s="11" t="inlineStr">
-        <is>
-          <t>CRQ000000248840</t>
-        </is>
-      </c>
-      <c r="L6" s="11" t="inlineStr">
-        <is>
-          <t>Muhammad Shahed</t>
-        </is>
-      </c>
+      <c r="B6" s="8" t="n"/>
+      <c r="C6" s="7" t="n"/>
+      <c r="D6" s="9" t="n"/>
+      <c r="E6" s="9" t="n"/>
+      <c r="F6" s="9" t="n"/>
+      <c r="G6" s="14" t="n"/>
+      <c r="H6" s="9" t="n"/>
+      <c r="I6" s="9" t="n"/>
+      <c r="J6" s="10" t="n"/>
+      <c r="K6" s="11" t="n"/>
+      <c r="L6" s="11" t="n"/>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="1">
       <c r="A7" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="inlineStr">
-        <is>
-          <t>28-Jul-20</t>
-        </is>
-      </c>
-      <c r="C7" s="7" t="inlineStr">
-        <is>
-          <t>Md. Masudur Rahman</t>
-        </is>
-      </c>
-      <c r="D7" s="9" t="inlineStr">
-        <is>
-          <t>Pinacle</t>
-        </is>
-      </c>
-      <c r="E7" s="9" t="inlineStr">
-        <is>
-          <t>MMU  changed</t>
-        </is>
-      </c>
-      <c r="F7" s="9" t="inlineStr">
-        <is>
-          <t>DHADB03,DHADB20</t>
-        </is>
-      </c>
-      <c r="G7" s="14" t="inlineStr">
-        <is>
-          <t>Service Effective</t>
-        </is>
-      </c>
-      <c r="H7" s="9" t="inlineStr">
-        <is>
-          <t>00:30 Minute</t>
-        </is>
-      </c>
-      <c r="I7" s="9" t="inlineStr">
-        <is>
-          <t>Dhaka</t>
-        </is>
-      </c>
-      <c r="J7" s="10" t="inlineStr">
-        <is>
-          <t>e.co_Dhaka Metro</t>
-        </is>
-      </c>
-      <c r="K7" s="11" t="inlineStr">
-        <is>
-          <t>CRQ000000248532</t>
-        </is>
-      </c>
-      <c r="L7" s="11" t="inlineStr">
-        <is>
-          <t>Muhammad Shahed</t>
-        </is>
-      </c>
+      <c r="B7" s="8" t="n"/>
+      <c r="C7" s="7" t="n"/>
+      <c r="D7" s="9" t="n"/>
+      <c r="E7" s="9" t="n"/>
+      <c r="F7" s="9" t="n"/>
+      <c r="G7" s="14" t="n"/>
+      <c r="H7" s="9" t="n"/>
+      <c r="I7" s="9" t="n"/>
+      <c r="J7" s="10" t="n"/>
+      <c r="K7" s="11" t="n"/>
+      <c r="L7" s="11" t="n"/>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="1">
       <c r="A8" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="inlineStr">
-        <is>
-          <t>28-Jul-20</t>
-        </is>
-      </c>
-      <c r="C8" s="7" t="inlineStr">
-        <is>
-          <t>Md. Masudur Rahman</t>
-        </is>
-      </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>CEP</t>
-        </is>
-      </c>
-      <c r="E8" s="9" t="inlineStr">
-        <is>
-          <t>PAT activity</t>
-        </is>
-      </c>
-      <c r="F8" s="9" t="inlineStr">
-        <is>
-          <t>DHLLB15,DHKTL18</t>
-        </is>
-      </c>
-      <c r="G8" s="14" t="inlineStr">
-        <is>
-          <t>Service Effective</t>
-        </is>
-      </c>
-      <c r="H8" s="9" t="inlineStr">
-        <is>
-          <t>00:30 Minute</t>
-        </is>
-      </c>
-      <c r="I8" s="9" t="inlineStr">
-        <is>
-          <t>Dhaka</t>
-        </is>
-      </c>
-      <c r="J8" s="10" t="inlineStr">
-        <is>
-          <t>e.co_Dhaka Metro</t>
-        </is>
-      </c>
-      <c r="K8" s="11" t="inlineStr">
-        <is>
-          <t>CRQ000000248535</t>
-        </is>
-      </c>
-      <c r="L8" s="11" t="inlineStr">
-        <is>
-          <t>Muhammad Shahed</t>
-        </is>
-      </c>
+      <c r="B8" s="8" t="n"/>
+      <c r="C8" s="7" t="n"/>
+      <c r="D8" s="9" t="n"/>
+      <c r="E8" s="9" t="n"/>
+      <c r="F8" s="9" t="n"/>
+      <c r="G8" s="14" t="n"/>
+      <c r="H8" s="9" t="n"/>
+      <c r="I8" s="9" t="n"/>
+      <c r="J8" s="10" t="n"/>
+      <c r="K8" s="11" t="n"/>
+      <c r="L8" s="11" t="n"/>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="1">
       <c r="A9" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="inlineStr">
-        <is>
-          <t>28-Jul-20</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="inlineStr">
-        <is>
-          <t>Md. Masudur Rahman</t>
-        </is>
-      </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>DHAKA_MODERNIZATION</t>
-        </is>
-      </c>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RAU Release Udate </t>
-        </is>
-      </c>
-      <c r="F9" s="9" t="inlineStr">
-        <is>
-          <t>DHKHL05,DHKHL74</t>
-        </is>
-      </c>
-      <c r="G9" s="14" t="inlineStr">
-        <is>
-          <t>Service Effective</t>
-        </is>
-      </c>
-      <c r="H9" s="9" t="inlineStr">
-        <is>
-          <t>00:30 Minute</t>
-        </is>
-      </c>
-      <c r="I9" s="9" t="inlineStr">
-        <is>
-          <t>Dhaka</t>
-        </is>
-      </c>
-      <c r="J9" s="10" t="inlineStr">
-        <is>
-          <t>e.co_Dhaka Metro</t>
-        </is>
-      </c>
-      <c r="K9" s="11" t="inlineStr">
-        <is>
-          <t>CRQ000000248538</t>
-        </is>
-      </c>
-      <c r="L9" s="11" t="inlineStr">
-        <is>
-          <t>Muhammad Shahed</t>
-        </is>
-      </c>
+      <c r="B9" s="8" t="n"/>
+      <c r="C9" s="7" t="n"/>
+      <c r="D9" s="9" t="n"/>
+      <c r="E9" s="9" t="n"/>
+      <c r="F9" s="9" t="n"/>
+      <c r="G9" s="14" t="n"/>
+      <c r="H9" s="9" t="n"/>
+      <c r="I9" s="9" t="n"/>
+      <c r="J9" s="10" t="n"/>
+      <c r="K9" s="11" t="n"/>
+      <c r="L9" s="11" t="n"/>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="1">
       <c r="A10" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="inlineStr">
-        <is>
-          <t>28-Jul-20</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="inlineStr">
-        <is>
-          <t>Md. Masudur Rahman</t>
-        </is>
-      </c>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>CEP</t>
-        </is>
-      </c>
-      <c r="E10" s="9" t="inlineStr">
-        <is>
-          <t>New Link instalation</t>
-        </is>
-      </c>
-      <c r="F10" s="9" t="inlineStr">
-        <is>
-          <t>DHTEJ07,DHTEJ15,DHKTL22</t>
-        </is>
-      </c>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>Non-Service Effective</t>
-        </is>
-      </c>
-      <c r="H10" s="9" t="inlineStr">
-        <is>
-          <t>00:00 Minute</t>
-        </is>
-      </c>
-      <c r="I10" s="9" t="inlineStr">
-        <is>
-          <t>Dhaka</t>
-        </is>
-      </c>
-      <c r="J10" s="10" t="inlineStr">
-        <is>
-          <t>e.co_Dhaka Metro</t>
-        </is>
-      </c>
-      <c r="K10" s="11" t="inlineStr">
-        <is>
-          <t>CRQ000000248543</t>
-        </is>
-      </c>
-      <c r="L10" s="11" t="inlineStr">
-        <is>
-          <t>Muhammad Shahed</t>
-        </is>
-      </c>
+      <c r="B10" s="8" t="n"/>
+      <c r="C10" s="7" t="n"/>
+      <c r="D10" s="9" t="n"/>
+      <c r="E10" s="9" t="n"/>
+      <c r="F10" s="9" t="n"/>
+      <c r="G10" s="14" t="n"/>
+      <c r="H10" s="9" t="n"/>
+      <c r="I10" s="9" t="n"/>
+      <c r="J10" s="10" t="n"/>
+      <c r="K10" s="11" t="n"/>
+      <c r="L10" s="11" t="n"/>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="1">
       <c r="A11" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="inlineStr">
-        <is>
-          <t>28-Jul-20</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="inlineStr">
-        <is>
-          <t>Md. Masudur Rahman</t>
-        </is>
-      </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>Padma_Colo</t>
-        </is>
-      </c>
-      <c r="E11" s="9" t="inlineStr">
-        <is>
-          <t>Traffic Shifting 1/1</t>
-        </is>
-      </c>
-      <c r="F11" s="9" t="inlineStr">
-        <is>
-          <t>HGSDR24,HGSDR04,HGBNC04,HGNBG05</t>
-        </is>
-      </c>
-      <c r="G11" s="14" t="inlineStr">
-        <is>
-          <t>Service Effective</t>
-        </is>
-      </c>
-      <c r="H11" s="9" t="inlineStr">
-        <is>
-          <t>00:30 Minute</t>
-        </is>
-      </c>
-      <c r="I11" s="9" t="inlineStr">
-        <is>
-          <t>Sylhet</t>
-        </is>
-      </c>
-      <c r="J11" s="10" t="inlineStr">
-        <is>
-          <t>e.co_Sylhet</t>
-        </is>
-      </c>
-      <c r="K11" s="11" t="inlineStr">
-        <is>
-          <t>CRQ000000248545</t>
-        </is>
-      </c>
-      <c r="L11" s="11" t="inlineStr">
-        <is>
-          <t>Muhammad Shahed</t>
-        </is>
-      </c>
+      <c r="B11" s="8" t="n"/>
+      <c r="C11" s="7" t="n"/>
+      <c r="D11" s="9" t="n"/>
+      <c r="E11" s="9" t="n"/>
+      <c r="F11" s="9" t="n"/>
+      <c r="G11" s="14" t="n"/>
+      <c r="H11" s="9" t="n"/>
+      <c r="I11" s="9" t="n"/>
+      <c r="J11" s="10" t="n"/>
+      <c r="K11" s="11" t="n"/>
+      <c r="L11" s="11" t="n"/>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="1">
       <c r="A12" s="7" t="n">

</xml_diff>

<commit_message>
Create Working Fine, Close Crusing, Cancel Working Fine
</commit_message>
<xml_diff>
--- a/data_driver/Change_Request_List.xlsx
+++ b/data_driver/Change_Request_List.xlsx
@@ -3,15 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Change_List" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Information" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Information" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="Barisal">Information!$V$2</definedName>
     <definedName name="Chittagong">Information!$Z$2</definedName>
@@ -338,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -420,6 +418,18 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -996,63 +1006,22 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
-    <sheetNames>
-      <sheetName val="Change_List"/>
-      <sheetName val="Information"/>
-      <sheetName val="My_NCR"/>
-      <sheetName val="Master_Change_Requirement"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L21" headerRowCount="1" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A1:L21"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="No" dataDxfId="11">
-      <calculatedColumnFormula>[1]!Table1[[#This Row],[No]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="11" name="Date" dataDxfId="10">
-      <calculatedColumnFormula>[1]!Table1[[#This Row],[Date]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" name="Project Coordinator" dataDxfId="9">
-      <calculatedColumnFormula>[1]!Table1[[#This Row],[Project Coordinator]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" name="Project Name" dataDxfId="8">
-      <calculatedColumnFormula>[1]!Table1[[#This Row],[Project Name]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" name="Change Activity" dataDxfId="7">
-      <calculatedColumnFormula>[1]!Table1[[#This Row],[Change Activity]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" name="Impact Site List" dataDxfId="6">
-      <calculatedColumnFormula>[1]!Table1[[#This Row],[Impact Site List]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" name="Service Type" dataDxfId="5">
-      <calculatedColumnFormula>[1]!Table1[[#This Row],[Service Type]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" name="Down Time" dataDxfId="4">
-      <calculatedColumnFormula>[1]!Table1[[#This Row],[Down Time]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" name="Site Group" dataDxfId="3">
-      <calculatedColumnFormula>[1]!Table1[[#This Row],[Site Group]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" name="Commercial Zone" dataDxfId="2">
-      <calculatedColumnFormula>[1]!Table1[[#This Row],[Commercial Zone]]</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" name="No" dataDxfId="11"/>
+    <tableColumn id="11" name="Date" dataDxfId="10"/>
+    <tableColumn id="2" name="Project Coordinator" dataDxfId="9"/>
+    <tableColumn id="3" name="Project Name" dataDxfId="8"/>
+    <tableColumn id="4" name="Change Activity" dataDxfId="7"/>
+    <tableColumn id="5" name="Impact Site List" dataDxfId="6"/>
+    <tableColumn id="6" name="Service Type" dataDxfId="5"/>
+    <tableColumn id="7" name="Down Time" dataDxfId="4"/>
+    <tableColumn id="8" name="Site Group" dataDxfId="3"/>
+    <tableColumn id="9" name="Commercial Zone" dataDxfId="2"/>
     <tableColumn id="10" name="NCR Number" dataDxfId="1"/>
-    <tableColumn id="12" name="Change Manager" dataDxfId="0">
-      <calculatedColumnFormula>[1]!Table1[[#This Row],[Change Manager]]</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="12" name="Change Manager" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1328,7 +1297,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1344,8 +1313,8 @@
     <col width="23.140625" bestFit="1" customWidth="1" style="25" min="10" max="10"/>
     <col width="16.85546875" bestFit="1" customWidth="1" style="3" min="11" max="11"/>
     <col width="17.42578125" bestFit="1" customWidth="1" style="25" min="12" max="12"/>
-    <col width="9.140625" customWidth="1" style="25" min="13" max="14"/>
-    <col width="9.140625" customWidth="1" style="25" min="15" max="16384"/>
+    <col width="9.140625" customWidth="1" style="25" min="13" max="20"/>
+    <col width="9.140625" customWidth="1" style="25" min="21" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" s="25">
@@ -1416,12 +1385,12 @@
       </c>
       <c r="B2" s="27" t="inlineStr">
         <is>
-          <t>12-Aug-20</t>
+          <t>16-Aug-20</t>
         </is>
       </c>
       <c r="C2" s="28" t="inlineStr">
         <is>
-          <t>Md. Masudur Rahman</t>
+          <t>KM Jiaul Islam Jibon</t>
         </is>
       </c>
       <c r="D2" s="29" t="inlineStr">
@@ -1431,12 +1400,12 @@
       </c>
       <c r="E2" s="29" t="inlineStr">
         <is>
-          <t>Dismantle activity</t>
+          <t>E1 Deletion</t>
         </is>
       </c>
       <c r="F2" s="29" t="inlineStr">
         <is>
-          <t>SYSDRD4,SYDKS28,SYGLP01,SYSDR86,SYSDR43,SYSDRC2</t>
+          <t>SNSDR01,SNSDR03,SYBLG05,SYBNB20,SYBNB40,SYBSW07,SYKNG02,SYSDRA7,SNSDR22,SNSDR25</t>
         </is>
       </c>
       <c r="G2" s="29" t="inlineStr">
@@ -1461,7 +1430,7 @@
       </c>
       <c r="K2" s="31" t="inlineStr">
         <is>
-          <t>CRQ000000250863</t>
+          <t>CRQ000000252000</t>
         </is>
       </c>
       <c r="L2" s="30" t="inlineStr">
@@ -1476,27 +1445,27 @@
       </c>
       <c r="B3" s="27" t="inlineStr">
         <is>
-          <t>11-Aug-20</t>
+          <t>15-Aug-20</t>
         </is>
       </c>
       <c r="C3" s="28" t="inlineStr">
         <is>
-          <t>Md. Rashekul Islam Raju</t>
+          <t>Md. Masudur Rahman</t>
         </is>
       </c>
       <c r="D3" s="29" t="inlineStr">
         <is>
-          <t>Project 964</t>
+          <t>Operational</t>
         </is>
       </c>
       <c r="E3" s="29" t="inlineStr">
         <is>
-          <t>GSM Antenna Optimization</t>
+          <t>Rectification &amp; Traffic shifting</t>
         </is>
       </c>
       <c r="F3" s="29" t="inlineStr">
         <is>
-          <t>DHSBB16</t>
+          <t>HGSDR24,HGSDR04, HGBNC04,HGNBG05</t>
         </is>
       </c>
       <c r="G3" s="29" t="inlineStr">
@@ -1506,22 +1475,22 @@
       </c>
       <c r="H3" s="29" t="inlineStr">
         <is>
-          <t>00:45 Minute</t>
+          <t>00:30 Minute</t>
         </is>
       </c>
       <c r="I3" s="29" t="inlineStr">
         <is>
-          <t>Dhaka</t>
+          <t>Sylhet</t>
         </is>
       </c>
       <c r="J3" s="29" t="inlineStr">
         <is>
-          <t>e.co_Dhaka Metro</t>
+          <t>e.co_Sylhet</t>
         </is>
       </c>
       <c r="K3" s="31" t="inlineStr">
         <is>
-          <t>CRQ000000250593</t>
+          <t>CRQ000000251948</t>
         </is>
       </c>
       <c r="L3" s="30" t="inlineStr">
@@ -1536,27 +1505,27 @@
       </c>
       <c r="B4" s="27" t="inlineStr">
         <is>
-          <t>11-Aug-20</t>
+          <t>15-Aug-20</t>
         </is>
       </c>
       <c r="C4" s="28" t="inlineStr">
         <is>
-          <t>KM Jiaul Islam Jibon</t>
+          <t>Md. Masudur Rahman</t>
         </is>
       </c>
       <c r="D4" s="29" t="inlineStr">
         <is>
-          <t>Dhaka-Modernization</t>
+          <t>NCCD AbisoIP</t>
         </is>
       </c>
       <c r="E4" s="33" t="inlineStr">
         <is>
-          <t>FE Configuration</t>
+          <t>Dismantle activity</t>
         </is>
       </c>
       <c r="F4" s="29" t="inlineStr">
         <is>
-          <t>TNDDR05,TNDDR15,TNKLH15,TNKLH16,TNMDP29</t>
+          <t>SYBNB22,SYBNB30,SNCTK01,SNCTK02,SNCTK04,SNCTK02,SNSDR03,SNSDR02,SYBNB15,SYBNB12</t>
         </is>
       </c>
       <c r="G4" s="29" t="inlineStr">
@@ -1571,17 +1540,17 @@
       </c>
       <c r="I4" s="29" t="inlineStr">
         <is>
-          <t>Mymensingh</t>
+          <t>Sylhet</t>
         </is>
       </c>
       <c r="J4" s="29" t="inlineStr">
         <is>
-          <t>e.co_Mymensingh</t>
+          <t>e.co_Sylhet</t>
         </is>
       </c>
       <c r="K4" s="31" t="inlineStr">
         <is>
-          <t>CRQ000000250595</t>
+          <t>CRQ000000251950</t>
         </is>
       </c>
       <c r="L4" s="30" t="inlineStr">
@@ -1596,27 +1565,27 @@
       </c>
       <c r="B5" s="27" t="inlineStr">
         <is>
-          <t>11-Aug-20</t>
+          <t>15-Aug-20</t>
         </is>
       </c>
       <c r="C5" s="28" t="inlineStr">
         <is>
-          <t>KM Jiaul Islam Jibon</t>
+          <t>Md. Masudur Rahman</t>
         </is>
       </c>
       <c r="D5" s="29" t="inlineStr">
         <is>
-          <t>Dhaka-Modernization</t>
+          <t>DHAKA_MODERNIZATION</t>
         </is>
       </c>
       <c r="E5" s="29" t="inlineStr">
         <is>
-          <t>FE Configuration</t>
+          <t>New Link instalation</t>
         </is>
       </c>
       <c r="F5" s="29" t="inlineStr">
         <is>
-          <t>DHMDP42,DHMDP47,DHMJH47,DHPTN16,DHPTN29,DHRMN04,DHRMN16,DHRMN26,DHRMN36</t>
+          <t>TNNGP12,TNKLH04</t>
         </is>
       </c>
       <c r="G5" s="29" t="inlineStr">
@@ -1631,17 +1600,17 @@
       </c>
       <c r="I5" s="29" t="inlineStr">
         <is>
-          <t>Dhaka</t>
+          <t>Mymensingh</t>
         </is>
       </c>
       <c r="J5" s="29" t="inlineStr">
         <is>
-          <t>e.co_Dhaka Metro</t>
+          <t>e.co_Mymensingh</t>
         </is>
       </c>
       <c r="K5" s="31" t="inlineStr">
         <is>
-          <t>CRQ000000250598</t>
+          <t>CRQ000000251952</t>
         </is>
       </c>
       <c r="L5" s="30" t="inlineStr">
@@ -1656,7 +1625,7 @@
       </c>
       <c r="B6" s="27" t="inlineStr">
         <is>
-          <t>11-Aug-20</t>
+          <t>15-Aug-20</t>
         </is>
       </c>
       <c r="C6" s="28" t="inlineStr">
@@ -1676,7 +1645,7 @@
       </c>
       <c r="F6" s="29" t="inlineStr">
         <is>
-          <t>MGGHR11,MGSBL11,MGSTR01,MNLHG02,MNLHG17,GPSDRS5,MNSDR46</t>
+          <t>DHMDP42,DHMDP47,DHMJH47,DHPTN16,DHPTN29,DHRMN04,DHRMN16,DHRMN26,DHRMN36</t>
         </is>
       </c>
       <c r="G6" s="29" t="inlineStr">
@@ -1696,12 +1665,12 @@
       </c>
       <c r="J6" s="29" t="inlineStr">
         <is>
-          <t>e.co_Dhaka North</t>
+          <t>e.co_Dhaka Metro</t>
         </is>
       </c>
       <c r="K6" s="30" t="inlineStr">
         <is>
-          <t>CRQ000000250602</t>
+          <t>CRQ000000251954</t>
         </is>
       </c>
       <c r="L6" s="30" t="inlineStr">
@@ -1716,7 +1685,7 @@
       </c>
       <c r="B7" s="27" t="inlineStr">
         <is>
-          <t>11-Aug-20</t>
+          <t>15-Aug-20</t>
         </is>
       </c>
       <c r="C7" s="28" t="inlineStr">
@@ -1726,17 +1695,17 @@
       </c>
       <c r="D7" s="29" t="inlineStr">
         <is>
-          <t xml:space="preserve">CEP_OEPX </t>
+          <t>Dhaka-Modernization</t>
         </is>
       </c>
       <c r="E7" s="29" t="inlineStr">
         <is>
-          <t>FE Configuration &amp; GE Shifting</t>
+          <t>FE Configuration</t>
         </is>
       </c>
       <c r="F7" s="29" t="inlineStr">
         <is>
-          <t>DHDHN07,DHRMN09</t>
+          <t>MGGHR11,MGSBL11,MGSTR01,MNLHG02,MNLHG17,GPSDRS5,MNSDR46</t>
         </is>
       </c>
       <c r="G7" s="29" t="inlineStr">
@@ -1756,12 +1725,12 @@
       </c>
       <c r="J7" s="29" t="inlineStr">
         <is>
-          <t>e.co_Dhaka Metro</t>
+          <t>e.co_Dhaka North</t>
         </is>
       </c>
       <c r="K7" s="30" t="inlineStr">
         <is>
-          <t>CRQ000000250604</t>
+          <t>CRQ000000251956</t>
         </is>
       </c>
       <c r="L7" s="30" t="inlineStr">
@@ -1776,27 +1745,27 @@
       </c>
       <c r="B8" s="27" t="inlineStr">
         <is>
-          <t>11-Aug-20</t>
+          <t>15-Aug-20</t>
         </is>
       </c>
       <c r="C8" s="28" t="inlineStr">
         <is>
-          <t>Md. Masudur Rahman</t>
+          <t>KM Jiaul Islam Jibon</t>
         </is>
       </c>
       <c r="D8" s="29" t="inlineStr">
         <is>
-          <t>Padma_Colo</t>
+          <t>CEP-OPEX</t>
         </is>
       </c>
       <c r="E8" s="29" t="inlineStr">
         <is>
-          <t>Rectification</t>
+          <t>FE Configuration &amp; GE Shifting</t>
         </is>
       </c>
       <c r="F8" s="29" t="inlineStr">
         <is>
-          <t>HGBNC04,HGNBG05</t>
+          <t>DHTEJ72,DHGUL74</t>
         </is>
       </c>
       <c r="G8" s="29" t="inlineStr">
@@ -1811,17 +1780,17 @@
       </c>
       <c r="I8" s="29" t="inlineStr">
         <is>
-          <t>Sylhet</t>
+          <t>Dhaka</t>
         </is>
       </c>
       <c r="J8" s="29" t="inlineStr">
         <is>
-          <t>e.co_Sylhet</t>
+          <t>e.co_Dhaka Metro</t>
         </is>
       </c>
       <c r="K8" s="30" t="inlineStr">
         <is>
-          <t>CRQ000000250607</t>
+          <t>CRQ000000251959</t>
         </is>
       </c>
       <c r="L8" s="30" t="inlineStr">
@@ -1834,121 +1803,33 @@
       <c r="A9" s="26" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="27" t="inlineStr">
-        <is>
-          <t>11-Aug-20</t>
-        </is>
-      </c>
-      <c r="C9" s="28" t="inlineStr">
-        <is>
-          <t>Md. Masudur Rahman</t>
-        </is>
-      </c>
-      <c r="D9" s="29" t="inlineStr">
-        <is>
-          <t>DHAKA_MODERNIZATION</t>
-        </is>
-      </c>
-      <c r="E9" s="29" t="inlineStr">
-        <is>
-          <t>Rectification</t>
-        </is>
-      </c>
-      <c r="F9" s="29" t="inlineStr">
-        <is>
-          <t>TNGPL01,TNGTL27</t>
-        </is>
-      </c>
-      <c r="G9" s="29" t="inlineStr">
-        <is>
-          <t>Service Effective</t>
-        </is>
-      </c>
-      <c r="H9" s="29" t="inlineStr">
-        <is>
-          <t>00:30 Minute</t>
-        </is>
-      </c>
-      <c r="I9" s="29" t="inlineStr">
-        <is>
-          <t>Mymensingh</t>
-        </is>
-      </c>
-      <c r="J9" s="29" t="inlineStr">
-        <is>
-          <t>e.co_Mymensingh</t>
-        </is>
-      </c>
-      <c r="K9" s="30" t="inlineStr">
-        <is>
-          <t>CRQ000000250609</t>
-        </is>
-      </c>
-      <c r="L9" s="30" t="inlineStr">
-        <is>
-          <t>Muhammad Shahed</t>
-        </is>
-      </c>
+      <c r="B9" s="27" t="n"/>
+      <c r="C9" s="28" t="n"/>
+      <c r="D9" s="29" t="n"/>
+      <c r="E9" s="29" t="n"/>
+      <c r="F9" s="29" t="n"/>
+      <c r="G9" s="29" t="n"/>
+      <c r="H9" s="29" t="n"/>
+      <c r="I9" s="29" t="n"/>
+      <c r="J9" s="29" t="n"/>
+      <c r="K9" s="30" t="n"/>
+      <c r="L9" s="30" t="n"/>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="25">
       <c r="A10" s="26" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="27" t="inlineStr">
-        <is>
-          <t>11-Aug-20</t>
-        </is>
-      </c>
-      <c r="C10" s="28" t="inlineStr">
-        <is>
-          <t>Md. Masudur Rahman</t>
-        </is>
-      </c>
-      <c r="D10" s="29" t="inlineStr">
-        <is>
-          <t>NCCD AbisoIP</t>
-        </is>
-      </c>
-      <c r="E10" s="29" t="inlineStr">
-        <is>
-          <t>Dismantle activity</t>
-        </is>
-      </c>
-      <c r="F10" s="29" t="inlineStr">
-        <is>
-          <t>SYGWN10,SYGWN13,SYGWN01,SYBNB02,SYSDR34,SYSDR08,SYSDR07,SYSDR13,SYSDR86,SYSDR43</t>
-        </is>
-      </c>
-      <c r="G10" s="29" t="inlineStr">
-        <is>
-          <t>Non-Service Effective</t>
-        </is>
-      </c>
-      <c r="H10" s="29" t="inlineStr">
-        <is>
-          <t>00:00 Minute</t>
-        </is>
-      </c>
-      <c r="I10" s="29" t="inlineStr">
-        <is>
-          <t>Sylhet</t>
-        </is>
-      </c>
-      <c r="J10" s="29" t="inlineStr">
-        <is>
-          <t>e.co_Sylhet</t>
-        </is>
-      </c>
-      <c r="K10" s="30" t="inlineStr">
-        <is>
-          <t>CRQ000000250612</t>
-        </is>
-      </c>
-      <c r="L10" s="30" t="inlineStr">
-        <is>
-          <t>Muhammad Shahed</t>
-        </is>
-      </c>
+      <c r="B10" s="27" t="n"/>
+      <c r="C10" s="28" t="n"/>
+      <c r="D10" s="29" t="n"/>
+      <c r="E10" s="29" t="n"/>
+      <c r="F10" s="29" t="n"/>
+      <c r="G10" s="29" t="n"/>
+      <c r="H10" s="29" t="n"/>
+      <c r="I10" s="29" t="n"/>
+      <c r="J10" s="29" t="n"/>
+      <c r="K10" s="30" t="n"/>
+      <c r="L10" s="30" t="n"/>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="25">
       <c r="A11" s="26" t="n">
@@ -1964,10 +1845,7 @@
       <c r="I11" s="29" t="n"/>
       <c r="J11" s="29" t="n"/>
       <c r="K11" s="31" t="n"/>
-      <c r="L11" s="30">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v/>
-      </c>
+      <c r="L11" s="30" t="n"/>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="25">
       <c r="A12" s="26" t="n">
@@ -1983,10 +1861,7 @@
       <c r="I12" s="29" t="n"/>
       <c r="J12" s="29" t="n"/>
       <c r="K12" s="31" t="n"/>
-      <c r="L12" s="30">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v/>
-      </c>
+      <c r="L12" s="30" t="n"/>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="25">
       <c r="A13" s="26" t="n">
@@ -2002,10 +1877,7 @@
       <c r="I13" s="29" t="n"/>
       <c r="J13" s="29" t="n"/>
       <c r="K13" s="31" t="n"/>
-      <c r="L13" s="30">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v/>
-      </c>
+      <c r="L13" s="30" t="n"/>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="25">
       <c r="A14" s="26" t="n">
@@ -2021,10 +1893,7 @@
       <c r="I14" s="29" t="n"/>
       <c r="J14" s="29" t="n"/>
       <c r="K14" s="31" t="n"/>
-      <c r="L14" s="30">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v/>
-      </c>
+      <c r="L14" s="30" t="n"/>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="25">
       <c r="A15" s="26" t="n">
@@ -2040,10 +1909,7 @@
       <c r="I15" s="29" t="n"/>
       <c r="J15" s="29" t="n"/>
       <c r="K15" s="31" t="n"/>
-      <c r="L15" s="30">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v/>
-      </c>
+      <c r="L15" s="30" t="n"/>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="25">
       <c r="A16" s="26" t="n">
@@ -2059,10 +1925,7 @@
       <c r="I16" s="29" t="n"/>
       <c r="J16" s="29" t="n"/>
       <c r="K16" s="31" t="n"/>
-      <c r="L16" s="30">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v/>
-      </c>
+      <c r="L16" s="30" t="n"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="25">
       <c r="A17" s="26" t="n">
@@ -2078,10 +1941,7 @@
       <c r="I17" s="29" t="n"/>
       <c r="J17" s="29" t="n"/>
       <c r="K17" s="31" t="n"/>
-      <c r="L17" s="30">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v/>
-      </c>
+      <c r="L17" s="30" t="n"/>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="25">
       <c r="A18" s="26" t="n">
@@ -2097,10 +1957,7 @@
       <c r="I18" s="29" t="n"/>
       <c r="J18" s="29" t="n"/>
       <c r="K18" s="31" t="n"/>
-      <c r="L18" s="30">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v/>
-      </c>
+      <c r="L18" s="30" t="n"/>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="25">
       <c r="A19" s="26" t="n">
@@ -2116,10 +1973,7 @@
       <c r="I19" s="29" t="n"/>
       <c r="J19" s="29" t="n"/>
       <c r="K19" s="31" t="n"/>
-      <c r="L19" s="30">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v/>
-      </c>
+      <c r="L19" s="30" t="n"/>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="25">
       <c r="A20" s="26" t="n">
@@ -2135,10 +1989,7 @@
       <c r="I20" s="29" t="n"/>
       <c r="J20" s="29" t="n"/>
       <c r="K20" s="31" t="n"/>
-      <c r="L20" s="30">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v/>
-      </c>
+      <c r="L20" s="30" t="n"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="25">
       <c r="A21" s="26" t="n">
@@ -2154,29 +2005,9 @@
       <c r="I21" s="29" t="n"/>
       <c r="J21" s="29" t="n"/>
       <c r="K21" s="32" t="n"/>
-      <c r="L21" s="30">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v/>
-      </c>
+      <c r="L21" s="30" t="n"/>
     </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation sqref="J3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>INDIRECT($I$4)</formula1>
-    </dataValidation>
-    <dataValidation sqref="J5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>INDIRECT($I$6)</formula1>
-    </dataValidation>
-    <dataValidation sqref="J4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>INDIRECT($I$5)</formula1>
-    </dataValidation>
-    <dataValidation sqref="J2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>INDIRECT($I$2)</formula1>
-    </dataValidation>
-    <dataValidation sqref="J6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>INDIRECT($I$7)</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0"/>
   <tableParts count="1">
@@ -2186,6 +2017,658 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="3.85546875" bestFit="1" customWidth="1" style="25" min="1" max="1"/>
+    <col width="7.7109375" bestFit="1" customWidth="1" style="25" min="2" max="2"/>
+    <col width="17.5703125" bestFit="1" customWidth="1" style="25" min="3" max="3"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="25" min="4" max="4"/>
+    <col width="74" bestFit="1" customWidth="1" style="25" min="5" max="5"/>
+    <col width="68.7109375" bestFit="1" customWidth="1" style="25" min="6" max="6"/>
+    <col width="15.140625" bestFit="1" customWidth="1" style="25" min="7" max="7"/>
+    <col width="10" bestFit="1" customWidth="1" style="25" min="8" max="8"/>
+    <col width="8.42578125" bestFit="1" customWidth="1" style="25" min="9" max="9"/>
+    <col width="13.42578125" bestFit="1" customWidth="1" style="25" min="10" max="10"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" style="25" min="11" max="11"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" style="25" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" customHeight="1" s="25">
+      <c r="A1" s="34" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="B1" s="35" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Project Coordinator</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Project Name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Change Activity</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Impact Site List</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Service Type</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Down Time</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Site Group</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Commercial Zone</t>
+        </is>
+      </c>
+      <c r="K1" s="36" t="inlineStr">
+        <is>
+          <t>NCR Number</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Change Manager</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="inlineStr">
+        <is>
+          <t>13-Aug-20</t>
+        </is>
+      </c>
+      <c r="C2" s="28" t="inlineStr">
+        <is>
+          <t>Prodip Biswas</t>
+        </is>
+      </c>
+      <c r="D2" s="29" t="inlineStr">
+        <is>
+          <t>L18CellAdd, Y2020</t>
+        </is>
+      </c>
+      <c r="E2" s="29" t="inlineStr">
+        <is>
+          <t>GSM &amp; RRU Swap</t>
+        </is>
+      </c>
+      <c r="F2" s="29" t="inlineStr">
+        <is>
+          <t>HGCNR16,SYZKG01,BMSDR31</t>
+        </is>
+      </c>
+      <c r="G2" s="29" t="inlineStr">
+        <is>
+          <t>Service Effective</t>
+        </is>
+      </c>
+      <c r="H2" s="29" t="inlineStr">
+        <is>
+          <t>00:30 Minute</t>
+        </is>
+      </c>
+      <c r="I2" s="29" t="inlineStr">
+        <is>
+          <t>Sylhet</t>
+        </is>
+      </c>
+      <c r="J2" s="29" t="inlineStr">
+        <is>
+          <t>e.co_Sylhet</t>
+        </is>
+      </c>
+      <c r="K2" s="31" t="inlineStr">
+        <is>
+          <t>CRQ000000251299</t>
+        </is>
+      </c>
+      <c r="L2" s="37" t="inlineStr">
+        <is>
+          <t>Sumon Kumar Biswas</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="27" t="inlineStr">
+        <is>
+          <t>13-Aug-20</t>
+        </is>
+      </c>
+      <c r="C3" s="28" t="inlineStr">
+        <is>
+          <t>KM Jiaul Islam Jibon</t>
+        </is>
+      </c>
+      <c r="D3" s="29" t="inlineStr">
+        <is>
+          <t>Dhaka-Modernization</t>
+        </is>
+      </c>
+      <c r="E3" s="29" t="inlineStr">
+        <is>
+          <t>FE Configuration</t>
+        </is>
+      </c>
+      <c r="F3" s="29" t="inlineStr">
+        <is>
+          <t>TNDDR05,TNDDR15,TNKLH15,TNKLH16,TNMDP29</t>
+        </is>
+      </c>
+      <c r="G3" s="29" t="inlineStr">
+        <is>
+          <t>Non-Service Effective</t>
+        </is>
+      </c>
+      <c r="H3" s="29" t="inlineStr">
+        <is>
+          <t>00:00 Minute</t>
+        </is>
+      </c>
+      <c r="I3" s="29" t="inlineStr">
+        <is>
+          <t>Mymensingh</t>
+        </is>
+      </c>
+      <c r="J3" s="29" t="inlineStr">
+        <is>
+          <t>e.co_Mymensingh</t>
+        </is>
+      </c>
+      <c r="K3" s="31" t="inlineStr">
+        <is>
+          <t>CRQ000000251313</t>
+        </is>
+      </c>
+      <c r="L3" s="37" t="inlineStr">
+        <is>
+          <t>Muhammad Shahed</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="27" t="inlineStr">
+        <is>
+          <t>13-Aug-20</t>
+        </is>
+      </c>
+      <c r="C4" s="28" t="inlineStr">
+        <is>
+          <t>KM Jiaul Islam Jibon</t>
+        </is>
+      </c>
+      <c r="D4" s="29" t="inlineStr">
+        <is>
+          <t>Dhaka-Modernization</t>
+        </is>
+      </c>
+      <c r="E4" s="29" t="inlineStr">
+        <is>
+          <t>FE Configuration</t>
+        </is>
+      </c>
+      <c r="F4" s="29" t="inlineStr">
+        <is>
+          <t>DHMDP42,DHMDP47,DHMJH47,DHPTN16,DHPTN29,DHRMN04,DHRMN16,DHRMN26,DHRMN36</t>
+        </is>
+      </c>
+      <c r="G4" s="29" t="inlineStr">
+        <is>
+          <t>Non-Service Effective</t>
+        </is>
+      </c>
+      <c r="H4" s="29" t="inlineStr">
+        <is>
+          <t>00:00 Minute</t>
+        </is>
+      </c>
+      <c r="I4" s="29" t="inlineStr">
+        <is>
+          <t>Dhaka</t>
+        </is>
+      </c>
+      <c r="J4" s="29" t="inlineStr">
+        <is>
+          <t>e.co_Dhaka Metro</t>
+        </is>
+      </c>
+      <c r="K4" s="31" t="inlineStr">
+        <is>
+          <t>CRQ000000251318</t>
+        </is>
+      </c>
+      <c r="L4" s="37" t="inlineStr">
+        <is>
+          <t>Muhammad Shahed</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="28" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="27" t="inlineStr">
+        <is>
+          <t>13-Aug-20</t>
+        </is>
+      </c>
+      <c r="C5" s="28" t="inlineStr">
+        <is>
+          <t>KM Jiaul Islam Jibon</t>
+        </is>
+      </c>
+      <c r="D5" s="29" t="inlineStr">
+        <is>
+          <t>Dhaka-Modernization</t>
+        </is>
+      </c>
+      <c r="E5" s="33" t="inlineStr">
+        <is>
+          <t>FE Configuration</t>
+        </is>
+      </c>
+      <c r="F5" s="29" t="inlineStr">
+        <is>
+          <t>MGGHR11,MGSBL11,MGSTR01,MNLHG02,MNLHG17,GPSDRS5,MNSDR46</t>
+        </is>
+      </c>
+      <c r="G5" s="29" t="inlineStr">
+        <is>
+          <t>Service Effective</t>
+        </is>
+      </c>
+      <c r="H5" s="29" t="inlineStr">
+        <is>
+          <t>00:00 Minute</t>
+        </is>
+      </c>
+      <c r="I5" s="29" t="inlineStr">
+        <is>
+          <t>Dhaka</t>
+        </is>
+      </c>
+      <c r="J5" s="29" t="inlineStr">
+        <is>
+          <t>e.co_Dhaka North</t>
+        </is>
+      </c>
+      <c r="K5" s="31" t="inlineStr">
+        <is>
+          <t>CRQ000000251321</t>
+        </is>
+      </c>
+      <c r="L5" s="37" t="inlineStr">
+        <is>
+          <t>Muhammad Shahed</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="28" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="inlineStr">
+        <is>
+          <t>13-Aug-20</t>
+        </is>
+      </c>
+      <c r="C6" s="28" t="inlineStr">
+        <is>
+          <t>Md. Masudur Rahman</t>
+        </is>
+      </c>
+      <c r="D6" s="29" t="inlineStr">
+        <is>
+          <t>Operational</t>
+        </is>
+      </c>
+      <c r="E6" s="29" t="inlineStr">
+        <is>
+          <t>Traffic shifting</t>
+        </is>
+      </c>
+      <c r="F6" s="29" t="inlineStr">
+        <is>
+          <t>HGSDR24,HGSDR04</t>
+        </is>
+      </c>
+      <c r="G6" s="29" t="inlineStr">
+        <is>
+          <t>Service Effective</t>
+        </is>
+      </c>
+      <c r="H6" s="29" t="inlineStr">
+        <is>
+          <t>00:30 Minute</t>
+        </is>
+      </c>
+      <c r="I6" s="29" t="inlineStr">
+        <is>
+          <t>Sylhet</t>
+        </is>
+      </c>
+      <c r="J6" s="29" t="inlineStr">
+        <is>
+          <t>e.co_Sylhet</t>
+        </is>
+      </c>
+      <c r="K6" s="31" t="inlineStr">
+        <is>
+          <t>CRQ000000251326</t>
+        </is>
+      </c>
+      <c r="L6" s="37" t="inlineStr">
+        <is>
+          <t>Muhammad Shahed</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="28" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="27" t="inlineStr">
+        <is>
+          <t>13-Aug-20</t>
+        </is>
+      </c>
+      <c r="C7" s="28" t="inlineStr">
+        <is>
+          <t>Md. Masudur Rahman</t>
+        </is>
+      </c>
+      <c r="D7" s="29" t="inlineStr">
+        <is>
+          <t>NCCD AbisoIP</t>
+        </is>
+      </c>
+      <c r="E7" s="29" t="inlineStr">
+        <is>
+          <t>Dismantle activity</t>
+        </is>
+      </c>
+      <c r="F7" s="29" t="inlineStr">
+        <is>
+          <t>HGCNR21,HGSDR02,HGNBG03,SYBLG04,HGNBG30,HGNBG04,HGSDR04</t>
+        </is>
+      </c>
+      <c r="G7" s="29" t="inlineStr">
+        <is>
+          <t>Non-Service Effective</t>
+        </is>
+      </c>
+      <c r="H7" s="29" t="inlineStr">
+        <is>
+          <t>00:00 Minute</t>
+        </is>
+      </c>
+      <c r="I7" s="29" t="inlineStr">
+        <is>
+          <t>Sylhet</t>
+        </is>
+      </c>
+      <c r="J7" s="29" t="inlineStr">
+        <is>
+          <t>e.co_Sylhet</t>
+        </is>
+      </c>
+      <c r="K7" s="30" t="inlineStr">
+        <is>
+          <t>CRQ000000251328</t>
+        </is>
+      </c>
+      <c r="L7" s="37" t="inlineStr">
+        <is>
+          <t>Muhammad Shahed</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="28" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="27" t="inlineStr">
+        <is>
+          <t>12-Aug-20</t>
+        </is>
+      </c>
+      <c r="C8" s="28" t="inlineStr">
+        <is>
+          <t>KM Jiaul Islam Jibon</t>
+        </is>
+      </c>
+      <c r="D8" s="29" t="inlineStr">
+        <is>
+          <t>Dhaka-Modernization</t>
+        </is>
+      </c>
+      <c r="E8" s="29" t="inlineStr">
+        <is>
+          <t>FE Configuration</t>
+        </is>
+      </c>
+      <c r="F8" s="29" t="inlineStr">
+        <is>
+          <t>TNDDR05,TNDDR15,TNKLH15,TNKLH16,TNMDP29</t>
+        </is>
+      </c>
+      <c r="G8" s="29" t="inlineStr">
+        <is>
+          <t>Non-Service Effective</t>
+        </is>
+      </c>
+      <c r="H8" s="29" t="inlineStr">
+        <is>
+          <t>00:00 Minute</t>
+        </is>
+      </c>
+      <c r="I8" s="29" t="inlineStr">
+        <is>
+          <t>Mymensingh</t>
+        </is>
+      </c>
+      <c r="J8" s="29" t="inlineStr">
+        <is>
+          <t>e.co_Mymensingh</t>
+        </is>
+      </c>
+      <c r="K8" s="31" t="inlineStr">
+        <is>
+          <t>CRQ000000251008</t>
+        </is>
+      </c>
+      <c r="L8" s="37" t="inlineStr">
+        <is>
+          <t>Muhammad Shahed</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="28" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="27" t="inlineStr">
+        <is>
+          <t>12-Aug-20</t>
+        </is>
+      </c>
+      <c r="C9" s="28" t="inlineStr">
+        <is>
+          <t>KM Jiaul Islam Jibon</t>
+        </is>
+      </c>
+      <c r="D9" s="29" t="inlineStr">
+        <is>
+          <t>Dhaka-Modernization</t>
+        </is>
+      </c>
+      <c r="E9" s="29" t="inlineStr">
+        <is>
+          <t>FE Configuration</t>
+        </is>
+      </c>
+      <c r="F9" s="29" t="inlineStr">
+        <is>
+          <t>DHMDP42,DHMDP47,DHMJH47,DHPTN16,DHPTN29,DHRMN04,DHRMN16,DHRMN26,DHRMN36</t>
+        </is>
+      </c>
+      <c r="G9" s="29" t="inlineStr">
+        <is>
+          <t>Non-Service Effective</t>
+        </is>
+      </c>
+      <c r="H9" s="29" t="inlineStr">
+        <is>
+          <t>00:00 Minute</t>
+        </is>
+      </c>
+      <c r="I9" s="29" t="inlineStr">
+        <is>
+          <t>Dhaka</t>
+        </is>
+      </c>
+      <c r="J9" s="29" t="inlineStr">
+        <is>
+          <t>e.co_Dhaka Metro</t>
+        </is>
+      </c>
+      <c r="K9" s="31" t="inlineStr">
+        <is>
+          <t>CRQ000000251011</t>
+        </is>
+      </c>
+      <c r="L9" s="37" t="inlineStr">
+        <is>
+          <t>Muhammad Shahed</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="28" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="27" t="inlineStr">
+        <is>
+          <t>12-Aug-20</t>
+        </is>
+      </c>
+      <c r="C10" s="28" t="inlineStr">
+        <is>
+          <t>KM Jiaul Islam Jibon</t>
+        </is>
+      </c>
+      <c r="D10" s="29" t="inlineStr">
+        <is>
+          <t>Dhaka-Modernization</t>
+        </is>
+      </c>
+      <c r="E10" s="33" t="inlineStr">
+        <is>
+          <t>FE Configuration</t>
+        </is>
+      </c>
+      <c r="F10" s="29" t="inlineStr">
+        <is>
+          <t>MGGHR11,MGSBL11,MGSTR01,MNLHG02,MNLHG17,GPSDRS5,MNSDR46</t>
+        </is>
+      </c>
+      <c r="G10" s="29" t="inlineStr">
+        <is>
+          <t>Service Effective</t>
+        </is>
+      </c>
+      <c r="H10" s="29" t="inlineStr">
+        <is>
+          <t>00:00 Minute</t>
+        </is>
+      </c>
+      <c r="I10" s="29" t="inlineStr">
+        <is>
+          <t>Dhaka</t>
+        </is>
+      </c>
+      <c r="J10" s="29" t="inlineStr">
+        <is>
+          <t>e.co_Dhaka North</t>
+        </is>
+      </c>
+      <c r="K10" s="31" t="inlineStr">
+        <is>
+          <t>CRQ000000251013</t>
+        </is>
+      </c>
+      <c r="L10" s="37" t="inlineStr">
+        <is>
+          <t>Muhammad Shahed</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="5">
+    <dataValidation sqref="J7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>INDIRECT($I$7)</formula1>
+    </dataValidation>
+    <dataValidation sqref="J8 J2:J3" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>INDIRECT($I$2)</formula1>
+    </dataValidation>
+    <dataValidation sqref="J10 J5" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>INDIRECT($I$5)</formula1>
+    </dataValidation>
+    <dataValidation sqref="J6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>INDIRECT($I$6)</formula1>
+    </dataValidation>
+    <dataValidation sqref="J9 J4" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>INDIRECT($I$4)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2323,7 +2806,7 @@
         <f>""&amp;A2</f>
         <v/>
       </c>
-      <c r="C2" s="34" t="n">
+      <c r="C2" s="38" t="n">
         <v>44016</v>
       </c>
       <c r="D2" s="7" t="n">
@@ -2419,7 +2902,7 @@
         <f>B2&amp;","&amp;A3</f>
         <v/>
       </c>
-      <c r="C3" s="35" t="n"/>
+      <c r="C3" s="39" t="n"/>
       <c r="D3" s="7" t="n">
         <v>0.4583333333333333</v>
       </c>
@@ -2477,7 +2960,7 @@
         <f>B3&amp;","&amp;A4</f>
         <v/>
       </c>
-      <c r="C4" s="35" t="n"/>
+      <c r="C4" s="39" t="n"/>
       <c r="D4" s="7" t="n">
         <v>0.4861111111111111</v>
       </c>
@@ -2531,7 +3014,7 @@
         <f>B4&amp;","&amp;A5</f>
         <v/>
       </c>
-      <c r="C5" s="35" t="n"/>
+      <c r="C5" s="39" t="n"/>
       <c r="D5" s="7" t="n">
         <v>0.7083333333333334</v>
       </c>
@@ -2566,7 +3049,7 @@
         <f>B5&amp;","&amp;A6</f>
         <v/>
       </c>
-      <c r="C6" s="36" t="n"/>
+      <c r="C6" s="40" t="n"/>
       <c r="D6" s="7" t="n">
         <v>0.75</v>
       </c>

</xml_diff>

<commit_message>
created,closed & cancelled change request successfully
</commit_message>
<xml_diff>
--- a/data_driver/Change_Request_List.xlsx
+++ b/data_driver/Change_Request_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\AutoBotBMCRemedy\data_driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B384E5E-E291-43BF-9038-DC9B4C9A20D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F50720D-5A37-481F-B1E0-4D112367BB37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change_List" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="158">
   <si>
     <t>No</t>
   </si>
@@ -74,25 +74,79 @@
     <t>Change Manager</t>
   </si>
   <si>
-    <t>30-Aug-20</t>
-  </si>
-  <si>
-    <t>Md. Shahadat Hossain</t>
-  </si>
-  <si>
-    <t>Padma Colocation Project</t>
-  </si>
-  <si>
-    <t>CPRI Cable &amp; RRU Swap 1/1</t>
-  </si>
-  <si>
-    <t>         SNDRI02,SNDRI05,SNDRI06,SNDRI07,SNDRI10</t>
+    <t>31-Aug-20</t>
+  </si>
+  <si>
+    <t>Md. Masudur Rahman</t>
+  </si>
+  <si>
+    <t>DHAKA_MODERNIZATION</t>
+  </si>
+  <si>
+    <t>New Link installation</t>
+  </si>
+  <si>
+    <t>MGSNG08,DHKGNT1</t>
+  </si>
+  <si>
+    <t>Non-Service Effective</t>
+  </si>
+  <si>
+    <t>00:00 Minute</t>
+  </si>
+  <si>
+    <t>Dhaka</t>
+  </si>
+  <si>
+    <t>e.co_Dhaka North</t>
+  </si>
+  <si>
+    <t>CRQ000000257523</t>
+  </si>
+  <si>
+    <t>Muhammad Shahed</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>DHBDDA7,DHTEJ15,DHTEJ07</t>
+  </si>
+  <si>
+    <t>e.co_Dhaka Metro</t>
+  </si>
+  <si>
+    <t>CRQ000000257526</t>
+  </si>
+  <si>
+    <t>Padma_Colo</t>
+  </si>
+  <si>
+    <t>BHCFN02,BHCFN26,BHLMN01,BHLMN15</t>
+  </si>
+  <si>
+    <t>Barisal</t>
+  </si>
+  <si>
+    <t>e.co_Barisal</t>
+  </si>
+  <si>
+    <t>CRQ000000257528</t>
+  </si>
+  <si>
+    <t>NCCD AbisoIP</t>
+  </si>
+  <si>
+    <t>Traffic Check for Traffic shiftng</t>
+  </si>
+  <si>
+    <t>HGNBG28,HGNBG08</t>
   </si>
   <si>
     <t>Service Effective</t>
   </si>
   <si>
-    <t>04:00 Hour</t>
+    <t>00:30 Minute</t>
   </si>
   <si>
     <t>Sylhet</t>
@@ -101,10 +155,13 @@
     <t>e.co_Sylhet</t>
   </si>
   <si>
-    <t>CRQ000000257325</t>
-  </si>
-  <si>
-    <t>Muhammad Shahed</t>
+    <t>CRQ000000257530</t>
+  </si>
+  <si>
+    <t>DHMDP30,DHMDP39</t>
+  </si>
+  <si>
+    <t>CRQ000000257532</t>
   </si>
   <si>
     <t>29-Aug-20</t>
@@ -122,66 +179,24 @@
     <t>SYGLP22,SYDKS25</t>
   </si>
   <si>
-    <t>00:30 Minute</t>
-  </si>
-  <si>
     <t>CRQ000000257020</t>
   </si>
   <si>
     <t>Sumon Kumar Biswas</t>
   </si>
   <si>
-    <t>Md. Masudur Rahman</t>
-  </si>
-  <si>
-    <t>DHAKA_MODERNIZATION</t>
-  </si>
-  <si>
-    <t>New Link installation</t>
-  </si>
-  <si>
-    <t>MGSNG08,DHKGNT1</t>
-  </si>
-  <si>
-    <t>Non-Service Effective</t>
-  </si>
-  <si>
-    <t>00:00 Minute</t>
-  </si>
-  <si>
-    <t>Dhaka</t>
-  </si>
-  <si>
-    <t>e.co_Dhaka North</t>
-  </si>
-  <si>
     <t>CRQ000000257022</t>
   </si>
   <si>
-    <t>CEP</t>
-  </si>
-  <si>
     <t>DHTEJ15,DHTEJ07,DHTIA32,DHTIA11</t>
   </si>
   <si>
-    <t>e.co_Dhaka Metro</t>
-  </si>
-  <si>
     <t>CRQ000000257024</t>
   </si>
   <si>
-    <t>Padma_Colo</t>
-  </si>
-  <si>
     <t>MDKLK01,BSMLD12,BHLMN01,BHLMN15</t>
   </si>
   <si>
-    <t>Barisal</t>
-  </si>
-  <si>
-    <t>e.co_Barisal</t>
-  </si>
-  <si>
     <t>CRQ000000257026</t>
   </si>
   <si>
@@ -194,9 +209,6 @@
     <t>CRQ000000257028</t>
   </si>
   <si>
-    <t>DHMDP30,DHMDP39</t>
-  </si>
-  <si>
     <t>CRQ000000257030</t>
   </si>
   <si>
@@ -234,9 +246,6 @@
   </si>
   <si>
     <t>CRQ000000257036</t>
-  </si>
-  <si>
-    <t>NCCD AbisoIP</t>
   </si>
   <si>
     <t>Garbage E1 Deletetion</t>
@@ -358,10 +367,19 @@
     <t>CRQ000000256041</t>
   </si>
   <si>
+    <t>Md. Shahadat Hossain</t>
+  </si>
+  <si>
+    <t>Padma Colocation Project</t>
+  </si>
+  <si>
     <t>CPRI Cable &amp; RRU Swap</t>
   </si>
   <si>
     <t>                 SNJGN20,SNDRI06,SNDRI07,SNDRI10</t>
+  </si>
+  <si>
+    <t>04:00 Hour</t>
   </si>
   <si>
     <t>New Link instalation</t>
@@ -1706,7 +1724,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,8 +1740,8 @@
     <col min="10" max="10" width="23.140625" style="25" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="13" max="42" width="9.140625" style="25" customWidth="1"/>
-    <col min="43" max="16384" width="9.140625" style="25"/>
+    <col min="13" max="43" width="9.140625" style="25" customWidth="1"/>
+    <col min="44" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1806,65 +1824,153 @@
       <c r="A3" s="26">
         <v>2</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="28"/>
+      <c r="B3" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <v>3</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="28"/>
+      <c r="B4" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="28"/>
+      <c r="B5" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
+      <c r="B6" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
@@ -2183,37 +2289,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2221,34 +2327,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="L3" s="35" t="s">
         <v>22</v>
@@ -2259,34 +2365,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>40</v>
-      </c>
       <c r="E4" s="31" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="J4" s="27" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="L4" s="35" t="s">
         <v>22</v>
@@ -2297,34 +2403,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="K5" s="29" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L5" s="35" t="s">
         <v>22</v>
@@ -2335,34 +2441,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="K6" s="28" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="L6" s="35" t="s">
         <v>22</v>
@@ -2373,34 +2479,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="27" t="s">
+      <c r="E7" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>52</v>
-      </c>
       <c r="G7" s="27" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="L7" s="35" t="s">
         <v>22</v>
@@ -2411,34 +2517,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I8" s="37" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J8" s="37" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="K8" s="39" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="L8" s="40" t="s">
         <v>22</v>
@@ -2449,34 +2555,34 @@
         <v>6</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="J9" s="27" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="K9" s="29" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="L9" s="35" t="s">
         <v>22</v>
@@ -2485,34 +2591,34 @@
     <row r="10" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37"/>
       <c r="B10" s="36" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I10" s="37" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="K10" s="39" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L10" s="40" t="s">
         <v>22</v>
@@ -2540,31 +2646,31 @@
         <v>44069</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I12" s="37" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K12" s="39" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="L12" s="40" t="s">
         <v>22</v>
@@ -2603,34 +2709,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J15" s="27" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K15" s="28" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="L15" s="35" t="s">
         <v>22</v>
@@ -2641,34 +2747,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H16" s="27" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K16" s="28" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L16" s="35" t="s">
         <v>22</v>
@@ -2679,34 +2785,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J17" s="27" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K17" s="28" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L17" s="35" t="s">
         <v>22</v>
@@ -2717,34 +2823,34 @@
         <v>17</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H18" s="27" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K18" s="28" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L18" s="35" t="s">
         <v>22</v>
@@ -2755,34 +2861,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K19" s="29" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="L19" s="35" t="s">
         <v>22</v>
@@ -2793,34 +2899,34 @@
         <v>1</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K22" s="29" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="L22" s="35" t="s">
         <v>22</v>
@@ -2831,34 +2937,34 @@
         <v>2</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="K23" s="29" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="L23" s="35" t="s">
         <v>22</v>
@@ -2869,37 +2975,37 @@
         <v>3</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H24" s="27" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K24" s="29" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="L24" s="35" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2907,37 +3013,37 @@
         <v>4</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H25" s="27" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I25" s="27" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K25" s="29" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="L25" s="35" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2945,34 +3051,34 @@
         <v>5</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H26" s="27" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="I26" s="27" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J26" s="27" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K26" s="28" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="L26" s="35" t="s">
         <v>22</v>
@@ -2983,34 +3089,34 @@
         <v>6</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H27" s="27" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="K27" s="29" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="L27" s="35" t="s">
         <v>22</v>
@@ -3021,34 +3127,34 @@
         <v>7</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E28" s="37" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="G28" s="37" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H28" s="37" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I28" s="37" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="J28" s="37" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="K28" s="39" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="L28" s="40" t="s">
         <v>22</v>
@@ -3059,34 +3165,34 @@
         <v>8</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E29" s="38" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="F29" s="37" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H29" s="37" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I29" s="37" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="J29" s="37" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="K29" s="39" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="L29" s="40" t="s">
         <v>22</v>
@@ -3100,31 +3206,31 @@
         <v>44069</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="F30" s="37" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G30" s="37" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H30" s="37" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I30" s="37" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="J30" s="37" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="K30" s="39" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="L30" s="40" t="s">
         <v>22</v>
@@ -3138,31 +3244,31 @@
         <v>44069</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="G31" s="37" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H31" s="37" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I31" s="37" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="J31" s="37" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="K31" s="39" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="L31" s="40" t="s">
         <v>22</v>
@@ -3176,31 +3282,31 @@
         <v>44069</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F32" s="37" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G32" s="37" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H32" s="37" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I32" s="37" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="J32" s="37" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K32" s="39" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="L32" s="40" t="s">
         <v>22</v>
@@ -3253,16 +3359,16 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -3274,42 +3380,42 @@
         <v>7</v>
       </c>
       <c r="U1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y1" s="13" t="s">
-        <v>19</v>
-      </c>
       <c r="Z1" s="13" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="AA1" s="13" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="AB1" s="13" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="AC1" s="13" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="AD1" s="13" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="AE1" s="13" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B2" s="12" t="str">
         <f>""&amp;A2</f>
@@ -3326,54 +3432,54 @@
         <v>07/04/2020 9:00 AM</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="U2" s="14" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="W2" s="14" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="X2" s="14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="Y2" s="14" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="Z2" s="14" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="AA2" s="14" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="AB2" s="14" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="AC2" s="14" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="AD2" s="14" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="AE2" s="14" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B3" s="12" t="str">
         <f t="shared" ref="B3:B11" si="0">B2&amp;","&amp;A3</f>
@@ -3388,26 +3494,26 @@
         <v>07/04/2020 11:00 AM</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="U3" s="14" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="V3" s="14"/>
       <c r="W3" s="14"/>
       <c r="X3" s="14"/>
       <c r="Y3" s="14"/>
       <c r="Z3" s="14" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="AA3" s="14"/>
       <c r="AB3" s="14"/>
@@ -3417,7 +3523,7 @@
     </row>
     <row r="4" spans="1:31" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B4" s="12" t="str">
         <f t="shared" si="0"/>
@@ -3432,24 +3538,24 @@
         <v>07/04/2020 11:40 AM</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="O4" s="21" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="U4" s="14" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="V4" s="14"/>
       <c r="W4" s="14"/>
       <c r="X4" s="14"/>
       <c r="Y4" s="14"/>
       <c r="Z4" s="14" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="AA4" s="14"/>
       <c r="AB4" s="14"/>
@@ -3459,7 +3565,7 @@
     </row>
     <row r="5" spans="1:31" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B5" s="12" t="str">
         <f t="shared" si="0"/>
@@ -3474,19 +3580,19 @@
         <v>07/04/2020 5:00 PM</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="4" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B6" s="12" t="str">
         <f t="shared" si="0"/>
@@ -3501,14 +3607,14 @@
         <v>07/04/2020 6:00 PM</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="O6" s="21" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -3518,11 +3624,11 @@
         <v>DHGUL10,DHGUL74,DHGUL76,DHMRP28,DHPLB19,</v>
       </c>
       <c r="O7" s="21" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -3534,7 +3640,7 @@
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
       <c r="Q8" s="4" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -3546,7 +3652,7 @@
       <c r="O9" s="22"/>
       <c r="P9" s="22"/>
       <c r="Q9" s="4" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -3556,11 +3662,11 @@
         <v>DHGUL10,DHGUL74,DHGUL76,DHMRP28,DHPLB19,,,,</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="P10" s="22"/>
       <c r="Q10" s="4" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -3575,31 +3681,31 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O12" s="23" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O13" s="23" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O14" s="23" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="U14" s="19"/>
       <c r="V14" s="20"/>
     </row>
     <row r="15" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O15" s="23" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="U15" s="19"/>
       <c r="V15" s="20"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O16" s="23" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="15:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Exporting LDMA LB completed
</commit_message>
<xml_diff>
--- a/data_driver/Change_Request_List.xlsx
+++ b/data_driver/Change_Request_List.xlsx
@@ -2018,8 +2018,8 @@
     <col width="15.7109375" bestFit="1" customWidth="1" style="41" min="10" max="10"/>
     <col width="16.7109375" bestFit="1" customWidth="1" style="3" min="11" max="11"/>
     <col width="17" bestFit="1" customWidth="1" style="41" min="12" max="12"/>
-    <col width="9.140625" customWidth="1" style="41" min="13" max="16"/>
-    <col width="9.140625" customWidth="1" style="41" min="17" max="16384"/>
+    <col width="9.140625" customWidth="1" style="41" min="13" max="17"/>
+    <col width="9.140625" customWidth="1" style="41" min="18" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" s="41">
@@ -2090,7 +2090,7 @@
       </c>
       <c r="B2" s="30" t="inlineStr">
         <is>
-          <t>02-Nov-20</t>
+          <t>03-Nov-20</t>
         </is>
       </c>
       <c r="C2" s="31" t="inlineStr">
@@ -2110,7 +2110,7 @@
       </c>
       <c r="F2" s="31" t="inlineStr">
         <is>
-          <t>SYKNG16,SYKNG07,SYGLP08</t>
+          <t>SYBNB21,SYBNB30,SYBNB34</t>
         </is>
       </c>
       <c r="G2" s="31" t="inlineStr">
@@ -2135,7 +2135,7 @@
       </c>
       <c r="K2" s="32" t="inlineStr">
         <is>
-          <t>CRQ000000280109</t>
+          <t>CRQ000000280378</t>
         </is>
       </c>
       <c r="L2" s="33" t="inlineStr">
@@ -2150,52 +2150,52 @@
       </c>
       <c r="B3" s="30" t="inlineStr">
         <is>
-          <t>02-Nov-20</t>
+          <t>03-Nov-20</t>
         </is>
       </c>
       <c r="C3" s="31" t="inlineStr">
         <is>
-          <t>KM Jiaul Islam Jibon_01847188948</t>
+          <t>Sobuz Ahmed_01841122538</t>
         </is>
       </c>
       <c r="D3" s="31" t="inlineStr">
         <is>
-          <t>NCCD AbisoIP P3</t>
+          <t>NCCD AbisoIP</t>
         </is>
       </c>
       <c r="E3" s="31" t="inlineStr">
         <is>
-          <t>E2E Lease Site Ping Test 1/1</t>
+          <t>E1 deletion &amp; Collect BTS Cable</t>
         </is>
       </c>
       <c r="F3" s="31" t="inlineStr">
         <is>
-          <t>FPSDR04,FPSDR05,FPSDR09,RJPNG19</t>
+          <t>SYSDRD2,SYSDRD3,SYSDRB8,SYSDRA2</t>
         </is>
       </c>
       <c r="G3" s="31" t="inlineStr">
         <is>
-          <t>Service Effective</t>
+          <t>Non-Service Effective</t>
         </is>
       </c>
       <c r="H3" s="31" t="inlineStr">
         <is>
-          <t>00:30 Minute</t>
+          <t>00:00 Minute</t>
         </is>
       </c>
       <c r="I3" s="31" t="inlineStr">
         <is>
-          <t>Kustia</t>
+          <t>Sylhet</t>
         </is>
       </c>
       <c r="J3" s="31" t="inlineStr">
         <is>
-          <t>e.co_Kustia</t>
+          <t>e.co_Sylhet</t>
         </is>
       </c>
       <c r="K3" s="32" t="inlineStr">
         <is>
-          <t>CRQ000000280112</t>
+          <t>CRQ000000280381</t>
         </is>
       </c>
       <c r="L3" s="33" t="inlineStr">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="B4" s="30" t="inlineStr">
         <is>
-          <t>02-Nov-20</t>
+          <t>03-Nov-20</t>
         </is>
       </c>
       <c r="C4" s="31" t="inlineStr">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="F4" s="31" t="inlineStr">
         <is>
-          <t>HGMDB19, MBJRI14, BMSDR24, BMSRL10</t>
+          <t>MBKML11, MBSML14, BMSDR24, BMSRL10</t>
         </is>
       </c>
       <c r="G4" s="31" t="inlineStr">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="K4" s="32" t="inlineStr">
         <is>
-          <t>CRQ000000280119</t>
+          <t>CRQ000000280386</t>
         </is>
       </c>
       <c r="L4" s="33" t="inlineStr">
@@ -2270,57 +2270,57 @@
       </c>
       <c r="B5" s="30" t="inlineStr">
         <is>
-          <t>02-Nov-20</t>
+          <t>03-Nov-20</t>
         </is>
       </c>
       <c r="C5" s="31" t="inlineStr">
         <is>
-          <t>Prodip Biswas_01841133479</t>
+          <t>Md. Masudur Rahman_01841122536</t>
         </is>
       </c>
       <c r="D5" s="31" t="inlineStr">
         <is>
-          <t>L18CellAdd, Y2020</t>
+          <t>DHAKA_MODERNIZATION</t>
         </is>
       </c>
       <c r="E5" s="31" t="inlineStr">
         <is>
-          <t>Take Print Screen from MBB</t>
+          <t>Rectification</t>
         </is>
       </c>
       <c r="F5" s="31" t="inlineStr">
         <is>
-          <t>BMNBG30,BMNNG05,BMNNG09,BMSDR54,BMSRL08,HGAZM09,MBSML28,SYBLG30</t>
+          <t>NKKND02,MYISG02</t>
         </is>
       </c>
       <c r="G5" s="31" t="inlineStr">
         <is>
-          <t>Non-Service Effective</t>
+          <t>Service Effective</t>
         </is>
       </c>
       <c r="H5" s="31" t="inlineStr">
         <is>
-          <t>00:00 Minute</t>
+          <t>00:30 Minute</t>
         </is>
       </c>
       <c r="I5" s="31" t="inlineStr">
         <is>
-          <t>Sylhet</t>
+          <t>Mymensingh</t>
         </is>
       </c>
       <c r="J5" s="31" t="inlineStr">
         <is>
-          <t>e.co_Sylhet</t>
+          <t>e.co_Mymensingh</t>
         </is>
       </c>
       <c r="K5" s="32" t="inlineStr">
         <is>
-          <t>CRQ000000280125</t>
+          <t>CRQ000000280388</t>
         </is>
       </c>
       <c r="L5" s="33" t="inlineStr">
         <is>
-          <t>Sumon Kumar Biswas</t>
+          <t>Muhammad Shahed</t>
         </is>
       </c>
     </row>
@@ -2330,37 +2330,37 @@
       </c>
       <c r="B6" s="30" t="inlineStr">
         <is>
-          <t>02-Nov-20</t>
+          <t>03-Nov-20</t>
         </is>
       </c>
       <c r="C6" s="31" t="inlineStr">
         <is>
-          <t>Prodip Biswas_01841133479</t>
+          <t>Md. Masudur Rahman_01841122536</t>
         </is>
       </c>
       <c r="D6" s="31" t="inlineStr">
         <is>
-          <t>L18CellAdd, Y2020</t>
+          <t>Padma_Colo</t>
         </is>
       </c>
       <c r="E6" s="31" t="inlineStr">
         <is>
-          <t>Take Print Screen from MBB</t>
+          <t>Rectification 1/1</t>
         </is>
       </c>
       <c r="F6" s="31" t="inlineStr">
         <is>
-          <t>SYBSW17,SYDKS18,SYDKS21,SYGLP20,SYGLP21,SYGWN13,SYGWN19SYJNT08</t>
+          <t>SYKNG05,SYSDR26,SYJNT03,SYJNT08,SYJNT02</t>
         </is>
       </c>
       <c r="G6" s="31" t="inlineStr">
         <is>
-          <t>Non-Service Effective</t>
+          <t>Service Effective</t>
         </is>
       </c>
       <c r="H6" s="31" t="inlineStr">
         <is>
-          <t>00:00 Minute</t>
+          <t>00:30 Minute</t>
         </is>
       </c>
       <c r="I6" s="31" t="inlineStr">
@@ -2375,12 +2375,12 @@
       </c>
       <c r="K6" s="32" t="inlineStr">
         <is>
-          <t>CRQ000000280128</t>
+          <t>CRQ000000280392</t>
         </is>
       </c>
       <c r="L6" s="33" t="inlineStr">
         <is>
-          <t>Sumon Kumar Biswas</t>
+          <t>Muhammad Shahed</t>
         </is>
       </c>
     </row>
@@ -2390,27 +2390,27 @@
       </c>
       <c r="B7" s="30" t="inlineStr">
         <is>
-          <t>02-Nov-20</t>
+          <t>03-Nov-20</t>
         </is>
       </c>
       <c r="C7" s="31" t="inlineStr">
         <is>
-          <t>Prodip Biswas_01841133479</t>
+          <t>Md. Masudur Rahman_01841122536</t>
         </is>
       </c>
       <c r="D7" s="31" t="inlineStr">
         <is>
-          <t>L18CellAdd, Y2020</t>
+          <t>DHAKA_MODERNIZATION</t>
         </is>
       </c>
       <c r="E7" s="31" t="inlineStr">
         <is>
-          <t>Take Print Screen from MBB</t>
+          <t>Dismantle Materials Return</t>
         </is>
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>SYKNG03,SYKNG04,SYKNG12,BMNBG21,SYCMP09</t>
+          <t>DHDHM33,DHDHM36,MNSNG08</t>
         </is>
       </c>
       <c r="G7" s="31" t="inlineStr">
@@ -2425,22 +2425,22 @@
       </c>
       <c r="I7" s="31" t="inlineStr">
         <is>
-          <t>Sylhet</t>
+          <t>Dhaka</t>
         </is>
       </c>
       <c r="J7" s="31" t="inlineStr">
         <is>
-          <t>e.co_Sylhet</t>
+          <t>e.co_Dhaka North</t>
         </is>
       </c>
       <c r="K7" s="32" t="inlineStr">
         <is>
-          <t>CRQ000000280132</t>
+          <t>CRQ000000280400</t>
         </is>
       </c>
       <c r="L7" s="33" t="inlineStr">
         <is>
-          <t>Sumon Kumar Biswas</t>
+          <t>Muhammad Shahed</t>
         </is>
       </c>
     </row>
@@ -2450,27 +2450,27 @@
       </c>
       <c r="B8" s="30" t="inlineStr">
         <is>
-          <t>02-Nov-20</t>
+          <t>03-Nov-20</t>
         </is>
       </c>
       <c r="C8" s="31" t="inlineStr">
         <is>
-          <t>Md. Shafiqur Rahman_01841122531</t>
+          <t>Md. Masudur Rahman_01841122536</t>
         </is>
       </c>
       <c r="D8" s="31" t="inlineStr">
         <is>
-          <t>Relocation</t>
+          <t>Finito</t>
         </is>
       </c>
       <c r="E8" s="31" t="inlineStr">
         <is>
-          <t>FE Configure, Site name change</t>
+          <t>Rectification</t>
         </is>
       </c>
       <c r="F8" s="31" t="inlineStr">
         <is>
-          <t>DHTIA08,DHSBG28</t>
+          <t>DHDHN41,DHTEJ23,DHTIA09,DHRMN05</t>
         </is>
       </c>
       <c r="G8" s="31" t="inlineStr">
@@ -2495,7 +2495,7 @@
       </c>
       <c r="K8" s="32" t="inlineStr">
         <is>
-          <t>CRQ000000280134</t>
+          <t>CRQ000000280403</t>
         </is>
       </c>
       <c r="L8" s="33" t="inlineStr">
@@ -2510,7 +2510,7 @@
       </c>
       <c r="B9" s="30" t="inlineStr">
         <is>
-          <t>02-Nov-20</t>
+          <t>03-Nov-20</t>
         </is>
       </c>
       <c r="C9" s="31" t="inlineStr">
@@ -2520,27 +2520,27 @@
       </c>
       <c r="D9" s="31" t="inlineStr">
         <is>
-          <t>Padma_Colo</t>
+          <t>NCCD AbisoIP</t>
         </is>
       </c>
       <c r="E9" s="31" t="inlineStr">
         <is>
-          <t>Slot Remove for alarm clear</t>
+          <t>Return Dismantle Materials</t>
         </is>
       </c>
       <c r="F9" s="31" t="inlineStr">
         <is>
-          <t>SYGWN03,SYJNT08,SYJNT02</t>
+          <t>SYSDRD4,SYSDR34,SYGWN03,SYGWN05,SYJNT03,SYJNT08,SYGWN01,SYDKS28,SYGLP01</t>
         </is>
       </c>
       <c r="G9" s="31" t="inlineStr">
         <is>
-          <t>Service Effective</t>
+          <t>Non-Service Effective</t>
         </is>
       </c>
       <c r="H9" s="31" t="inlineStr">
         <is>
-          <t>00:30 Minute</t>
+          <t>00:00 Minute</t>
         </is>
       </c>
       <c r="I9" s="31" t="inlineStr">
@@ -2555,7 +2555,7 @@
       </c>
       <c r="K9" s="33" t="inlineStr">
         <is>
-          <t>CRQ000000280140</t>
+          <t>CRQ000000280408</t>
         </is>
       </c>
       <c r="L9" s="33" t="inlineStr">
@@ -2570,7 +2570,7 @@
       </c>
       <c r="B10" s="30" t="inlineStr">
         <is>
-          <t>02-Nov-20</t>
+          <t>03-Nov-20</t>
         </is>
       </c>
       <c r="C10" s="31" t="inlineStr">
@@ -2580,42 +2580,42 @@
       </c>
       <c r="D10" s="31" t="inlineStr">
         <is>
-          <t>DHAKA_MODERNIZATION</t>
+          <t>NCCD AbisoIP</t>
         </is>
       </c>
       <c r="E10" s="31" t="inlineStr">
         <is>
-          <t>Rectification</t>
+          <t>Slot Remove for alarm clear</t>
         </is>
       </c>
       <c r="F10" s="31" t="inlineStr">
         <is>
-          <t>NKKND02,MYISG02</t>
+          <t>SYBNB42</t>
         </is>
       </c>
       <c r="G10" s="31" t="inlineStr">
         <is>
-          <t>Service Effective</t>
+          <t>Non-Service Effective</t>
         </is>
       </c>
       <c r="H10" s="31" t="inlineStr">
         <is>
-          <t>00:30 Minute</t>
+          <t>00:00 Minute</t>
         </is>
       </c>
       <c r="I10" s="31" t="inlineStr">
         <is>
-          <t>Mymensingh</t>
+          <t>Sylhet</t>
         </is>
       </c>
       <c r="J10" s="31" t="inlineStr">
         <is>
-          <t>e.co_Mymensingh</t>
+          <t>e.co_Sylhet</t>
         </is>
       </c>
       <c r="K10" s="33" t="inlineStr">
         <is>
-          <t>CRQ000000280148</t>
+          <t>CRQ000000280410</t>
         </is>
       </c>
       <c r="L10" s="33" t="inlineStr">
@@ -2630,7 +2630,7 @@
       </c>
       <c r="B11" s="30" t="inlineStr">
         <is>
-          <t>02-Nov-20</t>
+          <t>03-Nov-20</t>
         </is>
       </c>
       <c r="C11" s="31" t="inlineStr">
@@ -2640,17 +2640,17 @@
       </c>
       <c r="D11" s="31" t="inlineStr">
         <is>
-          <t>Padma_Colo</t>
+          <t>NCCD AbisoIP</t>
         </is>
       </c>
       <c r="E11" s="31" t="inlineStr">
         <is>
-          <t>Rectification 1/1</t>
+          <t>Traffic Shifting 1/1</t>
         </is>
       </c>
       <c r="F11" s="31" t="inlineStr">
         <is>
-          <t>SYKNG05,SYSDR26,SYJNT03,SYJNT08</t>
+          <t>TNNGP12,TNKLH04,JPISL14,SRSDR07</t>
         </is>
       </c>
       <c r="G11" s="31" t="inlineStr">
@@ -2665,17 +2665,17 @@
       </c>
       <c r="I11" s="31" t="inlineStr">
         <is>
-          <t>Sylhet</t>
+          <t>Mymensingh</t>
         </is>
       </c>
       <c r="J11" s="31" t="inlineStr">
         <is>
-          <t>e.co_Sylhet</t>
+          <t>e.co_Mymensingh</t>
         </is>
       </c>
       <c r="K11" s="33" t="inlineStr">
         <is>
-          <t>CRQ000000280152</t>
+          <t>CRQ000000280415</t>
         </is>
       </c>
       <c r="L11" s="33" t="inlineStr">
@@ -2690,7 +2690,7 @@
       </c>
       <c r="B12" s="30" t="inlineStr">
         <is>
-          <t>02-Nov-20</t>
+          <t>03-Nov-20</t>
         </is>
       </c>
       <c r="C12" s="31" t="inlineStr">
@@ -2710,7 +2710,7 @@
       </c>
       <c r="F12" s="31" t="inlineStr">
         <is>
-          <t>DHDHM33,DHDHM36,MNSNG08</t>
+          <t>DHKGNT1,MNLHG18,MNSRN18,MNSRK13,MNSRK16,NGSNG11,NGSNG20</t>
         </is>
       </c>
       <c r="G12" s="31" t="inlineStr">
@@ -2730,12 +2730,12 @@
       </c>
       <c r="J12" s="31" t="inlineStr">
         <is>
-          <t>e.co_Dhaka North</t>
+          <t>e.co_Dhaka South</t>
         </is>
       </c>
       <c r="K12" s="33" t="inlineStr">
         <is>
-          <t>CRQ000000280159</t>
+          <t>CRQ000000280417</t>
         </is>
       </c>
       <c r="L12" s="33" t="inlineStr">
@@ -2750,7 +2750,7 @@
       </c>
       <c r="B13" s="30" t="inlineStr">
         <is>
-          <t>02-Nov-20</t>
+          <t>03-Nov-20</t>
         </is>
       </c>
       <c r="C13" s="31" t="inlineStr">
@@ -2760,17 +2760,17 @@
       </c>
       <c r="D13" s="31" t="inlineStr">
         <is>
-          <t>Finito</t>
+          <t>Padma_Colo</t>
         </is>
       </c>
       <c r="E13" s="31" t="inlineStr">
         <is>
-          <t>Rectification</t>
+          <t>Traffic shifting 1/1</t>
         </is>
       </c>
       <c r="F13" s="31" t="inlineStr">
         <is>
-          <t>DHDHN41,DHTEJ23,DHTIA09,DHRMN05</t>
+          <t>MBJRI11,MBJRI10</t>
         </is>
       </c>
       <c r="G13" s="31" t="inlineStr">
@@ -2785,17 +2785,17 @@
       </c>
       <c r="I13" s="31" t="inlineStr">
         <is>
-          <t>Dhaka</t>
+          <t>Sylhet</t>
         </is>
       </c>
       <c r="J13" s="31" t="inlineStr">
         <is>
-          <t>e.co_Dhaka Metro</t>
+          <t>e.co_Sylhet</t>
         </is>
       </c>
       <c r="K13" s="32" t="inlineStr">
         <is>
-          <t>CRQ000000280164</t>
+          <t>CRQ000000280423</t>
         </is>
       </c>
       <c r="L13" s="33" t="inlineStr">
@@ -2808,81 +2808,301 @@
       <c r="A14" s="29" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="30" t="n"/>
-      <c r="C14" s="31" t="n"/>
-      <c r="D14" s="31" t="n"/>
-      <c r="E14" s="31" t="n"/>
-      <c r="F14" s="31" t="n"/>
-      <c r="G14" s="31" t="n"/>
-      <c r="H14" s="31" t="n"/>
-      <c r="I14" s="31" t="n"/>
-      <c r="J14" s="31" t="n"/>
-      <c r="K14" s="32" t="n"/>
-      <c r="L14" s="33" t="n"/>
+      <c r="B14" s="30" t="inlineStr">
+        <is>
+          <t>03-Nov-20</t>
+        </is>
+      </c>
+      <c r="C14" s="31" t="inlineStr">
+        <is>
+          <t>Md. Rashekul Islam Raju_01841133472</t>
+        </is>
+      </c>
+      <c r="D14" s="31" t="inlineStr">
+        <is>
+          <t>MW antenna optimization</t>
+        </is>
+      </c>
+      <c r="E14" s="31" t="inlineStr">
+        <is>
+          <t>MW  Inactive antenna Dismantle</t>
+        </is>
+      </c>
+      <c r="F14" s="31" t="inlineStr">
+        <is>
+          <t>HGSDR02</t>
+        </is>
+      </c>
+      <c r="G14" s="31" t="inlineStr">
+        <is>
+          <t>Non-Service Effective</t>
+        </is>
+      </c>
+      <c r="H14" s="31" t="inlineStr">
+        <is>
+          <t>00:00 Minute</t>
+        </is>
+      </c>
+      <c r="I14" s="31" t="inlineStr">
+        <is>
+          <t>Sylhet</t>
+        </is>
+      </c>
+      <c r="J14" s="31" t="inlineStr">
+        <is>
+          <t>e.co_Sylhet</t>
+        </is>
+      </c>
+      <c r="K14" s="32" t="inlineStr">
+        <is>
+          <t>CRQ000000280428</t>
+        </is>
+      </c>
+      <c r="L14" s="33" t="inlineStr">
+        <is>
+          <t>Muhammad Shahed</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="41">
       <c r="A15" s="29" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="30" t="n"/>
-      <c r="C15" s="31" t="n"/>
-      <c r="D15" s="31" t="n"/>
-      <c r="E15" s="31" t="n"/>
-      <c r="F15" s="31" t="n"/>
-      <c r="G15" s="31" t="n"/>
-      <c r="H15" s="31" t="n"/>
-      <c r="I15" s="31" t="n"/>
-      <c r="J15" s="31" t="n"/>
-      <c r="K15" s="32" t="n"/>
-      <c r="L15" s="33" t="n"/>
+      <c r="B15" s="30" t="inlineStr">
+        <is>
+          <t>03-Nov-20</t>
+        </is>
+      </c>
+      <c r="C15" s="31" t="inlineStr">
+        <is>
+          <t>Md. Rashekul Islam Raju_01841133472</t>
+        </is>
+      </c>
+      <c r="D15" s="31" t="inlineStr">
+        <is>
+          <t>Y2020 Capacity Expansion Cell Split</t>
+        </is>
+      </c>
+      <c r="E15" s="31" t="inlineStr">
+        <is>
+          <t>GSM antenna  Swap by10Port ANT</t>
+        </is>
+      </c>
+      <c r="F15" s="31" t="inlineStr">
+        <is>
+          <t>NGSNG63, NGSNG68</t>
+        </is>
+      </c>
+      <c r="G15" s="31" t="inlineStr">
+        <is>
+          <t>Service Effective</t>
+        </is>
+      </c>
+      <c r="H15" s="31" t="inlineStr">
+        <is>
+          <t>00:45 Minute</t>
+        </is>
+      </c>
+      <c r="I15" s="31" t="inlineStr">
+        <is>
+          <t>Dhaka</t>
+        </is>
+      </c>
+      <c r="J15" s="31" t="inlineStr">
+        <is>
+          <t>e.co_Dhaka South</t>
+        </is>
+      </c>
+      <c r="K15" s="32" t="inlineStr">
+        <is>
+          <t>CRQ000000280432</t>
+        </is>
+      </c>
+      <c r="L15" s="33" t="inlineStr">
+        <is>
+          <t>Muhammad Shahed</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="41">
       <c r="A16" s="29" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="30" t="n"/>
-      <c r="C16" s="31" t="n"/>
-      <c r="D16" s="31" t="n"/>
-      <c r="E16" s="31" t="n"/>
-      <c r="F16" s="31" t="n"/>
-      <c r="G16" s="31" t="n"/>
-      <c r="H16" s="31" t="n"/>
-      <c r="I16" s="31" t="n"/>
-      <c r="J16" s="31" t="n"/>
-      <c r="K16" s="32" t="n"/>
-      <c r="L16" s="33" t="n"/>
+      <c r="B16" s="30" t="inlineStr">
+        <is>
+          <t>03-Nov-20</t>
+        </is>
+      </c>
+      <c r="C16" s="31" t="inlineStr">
+        <is>
+          <t>Md. Rashekul Islam Raju_01841133472</t>
+        </is>
+      </c>
+      <c r="D16" s="31" t="inlineStr">
+        <is>
+          <t>GSM antenna optimization</t>
+        </is>
+      </c>
+      <c r="E16" s="31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GSM antenna  Swap </t>
+        </is>
+      </c>
+      <c r="F16" s="31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                                  SYZKG14</t>
+        </is>
+      </c>
+      <c r="G16" s="31" t="inlineStr">
+        <is>
+          <t>Service Effective</t>
+        </is>
+      </c>
+      <c r="H16" s="31" t="inlineStr">
+        <is>
+          <t>00:45 Minute</t>
+        </is>
+      </c>
+      <c r="I16" s="31" t="inlineStr">
+        <is>
+          <t>Sylhet</t>
+        </is>
+      </c>
+      <c r="J16" s="31" t="inlineStr">
+        <is>
+          <t>e.co_Sylhet</t>
+        </is>
+      </c>
+      <c r="K16" s="32" t="inlineStr">
+        <is>
+          <t>CRQ000000280439</t>
+        </is>
+      </c>
+      <c r="L16" s="33" t="inlineStr">
+        <is>
+          <t>Muhammad Shahed</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="41">
       <c r="A17" s="29" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="30" t="n"/>
-      <c r="C17" s="31" t="n"/>
-      <c r="D17" s="31" t="n"/>
-      <c r="E17" s="31" t="n"/>
-      <c r="F17" s="31" t="n"/>
-      <c r="G17" s="31" t="n"/>
-      <c r="H17" s="31" t="n"/>
-      <c r="I17" s="31" t="n"/>
-      <c r="J17" s="31" t="n"/>
-      <c r="K17" s="32" t="n"/>
-      <c r="L17" s="33" t="n"/>
+      <c r="B17" s="30" t="inlineStr">
+        <is>
+          <t>03-Nov-20</t>
+        </is>
+      </c>
+      <c r="C17" s="31" t="inlineStr">
+        <is>
+          <t>Md. Rashekul Islam Raju_01841133472</t>
+        </is>
+      </c>
+      <c r="D17" s="31" t="inlineStr">
+        <is>
+          <t>GSM antenna optimization</t>
+        </is>
+      </c>
+      <c r="E17" s="31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GSM antenna  Swap </t>
+        </is>
+      </c>
+      <c r="F17" s="31" t="inlineStr">
+        <is>
+          <t>DHTIA01,DHGULD9</t>
+        </is>
+      </c>
+      <c r="G17" s="31" t="inlineStr">
+        <is>
+          <t>Service Effective</t>
+        </is>
+      </c>
+      <c r="H17" s="31" t="inlineStr">
+        <is>
+          <t>00:45 Minute</t>
+        </is>
+      </c>
+      <c r="I17" s="31" t="inlineStr">
+        <is>
+          <t>Dhaka</t>
+        </is>
+      </c>
+      <c r="J17" s="31" t="inlineStr">
+        <is>
+          <t>e.co_Dhaka Metro</t>
+        </is>
+      </c>
+      <c r="K17" s="32" t="inlineStr">
+        <is>
+          <t>CRQ000000280444</t>
+        </is>
+      </c>
+      <c r="L17" s="33" t="inlineStr">
+        <is>
+          <t>Muhammad Shahed</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="41">
       <c r="A18" s="29" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="30" t="n"/>
-      <c r="C18" s="31" t="n"/>
-      <c r="D18" s="31" t="n"/>
-      <c r="E18" s="31" t="n"/>
-      <c r="F18" s="31" t="n"/>
-      <c r="G18" s="31" t="n"/>
-      <c r="H18" s="31" t="n"/>
-      <c r="I18" s="31" t="n"/>
-      <c r="J18" s="31" t="n"/>
-      <c r="K18" s="32" t="n"/>
-      <c r="L18" s="33" t="n"/>
+      <c r="B18" s="30" t="inlineStr">
+        <is>
+          <t>03-Nov-20</t>
+        </is>
+      </c>
+      <c r="C18" s="31" t="inlineStr">
+        <is>
+          <t>Md. Rashekul Islam Raju_01841133472</t>
+        </is>
+      </c>
+      <c r="D18" s="31" t="inlineStr">
+        <is>
+          <t>MW antenna optimization</t>
+        </is>
+      </c>
+      <c r="E18" s="31" t="inlineStr">
+        <is>
+          <t>MW  Inactive antenna Dismantle</t>
+        </is>
+      </c>
+      <c r="F18" s="31" t="inlineStr">
+        <is>
+          <t>DHKHL26,DHKHL74</t>
+        </is>
+      </c>
+      <c r="G18" s="31" t="inlineStr">
+        <is>
+          <t>Non-Service Effective</t>
+        </is>
+      </c>
+      <c r="H18" s="31" t="inlineStr">
+        <is>
+          <t>00:00 Minute</t>
+        </is>
+      </c>
+      <c r="I18" s="31" t="inlineStr">
+        <is>
+          <t>Dhaka</t>
+        </is>
+      </c>
+      <c r="J18" s="31" t="inlineStr">
+        <is>
+          <t>e.co_Dhaka Metro</t>
+        </is>
+      </c>
+      <c r="K18" s="32" t="inlineStr">
+        <is>
+          <t>CRQ000000280449</t>
+        </is>
+      </c>
+      <c r="L18" s="33" t="inlineStr">
+        <is>
+          <t>Muhammad Shahed</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="41">
       <c r="A19" s="29" t="n">
@@ -3543,8 +3763,8 @@
     <col width="18" bestFit="1" customWidth="1" style="41" min="10" max="10"/>
     <col width="21.7109375" bestFit="1" customWidth="1" style="41" min="11" max="11"/>
     <col width="17.42578125" bestFit="1" customWidth="1" style="41" min="12" max="12"/>
-    <col width="9.140625" customWidth="1" style="41" min="13" max="17"/>
-    <col width="9.140625" customWidth="1" style="41" min="18" max="16384"/>
+    <col width="9.140625" customWidth="1" style="41" min="13" max="18"/>
+    <col width="9.140625" customWidth="1" style="41" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="41">

</xml_diff>